<commit_message>
Export --> Remarks : file updated with tc no - 23,24,25,26
</commit_message>
<xml_diff>
--- a/TCS_NEWUI-Export.xlsx
+++ b/TCS_NEWUI-Export.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="12240"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="12240" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
     <definedName name="test" localSheetId="2">#REF!</definedName>
     <definedName name="test">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="125725"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="232">
   <si>
     <t>Test Case Result Modules-Wise</t>
   </si>
@@ -677,16 +677,6 @@
     <t>Verify Pivot</t>
   </si>
   <si>
-    <t>User should be able to see following things on Pivot
-1. Pivot Bulk Actions button
-2. Pivot Options button
-3. Class,company &amp; division column in pivot
-4. All categories in pivot</t>
-  </si>
-  <si>
-    <t>Click Pivot Bulk Actions button</t>
-  </si>
-  <si>
     <t>List should be open &amp; user should be able to see following things
 1. Download Grid (Default Enabled)
 2. Create analert (Default Disabled)
@@ -748,6 +738,83 @@
   </si>
   <si>
     <t>US:WEB-7387_TC 24</t>
+  </si>
+  <si>
+    <t>Verify Exported video file should not be exported as Image</t>
+  </si>
+  <si>
+    <t>SMRT-8045</t>
+  </si>
+  <si>
+    <t>TC25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify Help Center link in exported excels and PPT should be redirects to new help link </t>
+  </si>
+  <si>
+    <t>SMRT-7944</t>
+  </si>
+  <si>
+    <t>US:WEB-7387_TC 25</t>
+  </si>
+  <si>
+    <t>TC26</t>
+  </si>
+  <si>
+    <t>Ac : Brand - QA Testing weekly report</t>
+  </si>
+  <si>
+    <t>Click on search options</t>
+  </si>
+  <si>
+    <t>Select "Online video" option from media</t>
+  </si>
+  <si>
+    <t>Click on apply button</t>
+  </si>
+  <si>
+    <t>"Online video" media type data should be displayed in AgGrid</t>
+  </si>
+  <si>
+    <t>Now select any record and click on Export button</t>
+  </si>
+  <si>
+    <t>Export window should be open</t>
+  </si>
+  <si>
+    <t>Select Creative Asset option &amp; click on send buton</t>
+  </si>
+  <si>
+    <t>1. File should be Exported
+2. Extract the expored file &amp; open the folder
+3. Exported file should not be image</t>
+  </si>
+  <si>
+    <t>Click Download options</t>
+  </si>
+  <si>
+    <t>User should be able to see following things on Pivot
+1. Download options button
+2. Pivot Options button
+3. Class,company &amp; division column in pivot
+4. All categories in pivot</t>
+  </si>
+  <si>
+    <t>US:WEB-7387_TC 26</t>
+  </si>
+  <si>
+    <t>Click on Export button then Select option Ad list XLS &amp; Click on send button</t>
+  </si>
+  <si>
+    <t>1. File should be exported
+2. Open the file and verify help link should be redirect to "https://help.www2.numerator.com/en/"</t>
+  </si>
+  <si>
+    <t>Now Click on Export button then Select option 
+"1 Creative / Slide" &amp; click on send button</t>
+  </si>
+  <si>
+    <t>We have ticket for old help link is displayed in PPT file</t>
   </si>
 </sst>
 </file>
@@ -856,7 +923,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1646,6 +1713,15 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="11" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="32" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="33" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="34" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="19" borderId="32" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1663,15 +1739,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="20" borderId="34" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="32" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="33" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="34" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="12" borderId="13" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1751,7 +1818,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout>
@@ -1762,7 +1828,7 @@
           <c:x val="5.3923741222529187E-2"/>
           <c:y val="0.14185650994577867"/>
           <c:w val="0.90694002510216154"/>
-          <c:h val="0.75521895211321832"/>
+          <c:h val="0.75521895211321866"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -1927,7 +1993,7 @@
                   <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1</c:v>
@@ -1944,12 +2010,11 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="86194432"/>
-        <c:axId val="86204416"/>
+        <c:axId val="52209152"/>
+        <c:axId val="52210688"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="86194432"/>
+        <c:axId val="52209152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1968,14 +2033,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="86204416"/>
+        <c:crossAx val="52210688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="86204416"/>
+        <c:axId val="52210688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1983,7 +2048,7 @@
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="86194432"/>
+        <c:crossAx val="52209152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2003,7 +2068,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000511" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000511" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000544" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000544" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2036,7 +2101,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:view3D>
       <c:rotX val="30"/>
@@ -2050,8 +2114,8 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="3.8831278392536694E-2"/>
-          <c:y val="0.14624350369603384"/>
-          <c:w val="0.92496729254319709"/>
+          <c:y val="0.14624350369603395"/>
+          <c:w val="0.92496729254319776"/>
           <c:h val="0.69766331701963369"/>
         </c:manualLayout>
       </c:layout>
@@ -2195,8 +2259,8 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.270891046791853"/>
-          <c:y val="0.88141746683253497"/>
-          <c:w val="0.42791036796598092"/>
+          <c:y val="0.88141746683253452"/>
+          <c:w val="0.42791036796598136"/>
           <c:h val="7.1280252974084315E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -2216,7 +2280,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000355" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000355" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000389" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000389" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
@@ -2234,9 +2298,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.27595722641494741"/>
-          <c:y val="7.1365887012686369E-2"/>
-          <c:w val="0.29672375522792599"/>
-          <c:h val="0.85466509216403819"/>
+          <c:y val="7.136588701268641E-2"/>
+          <c:w val="0.29672375522792616"/>
+          <c:h val="0.85466509216403874"/>
         </c:manualLayout>
       </c:layout>
       <c:pieChart>
@@ -2343,7 +2407,7 @@
                   <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1</c:v>
@@ -2360,7 +2424,6 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls/>
         <c:firstSliceAng val="0"/>
       </c:pieChart>
       <c:spPr>
@@ -2441,8 +2504,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.72165251246917417"/>
-          <c:y val="3.6083951617898579E-3"/>
+          <c:x val="0.72165251246917506"/>
+          <c:y val="3.6083951617898601E-3"/>
           <c:w val="0.24112408909611374"/>
           <c:h val="0.95693837006674254"/>
         </c:manualLayout>
@@ -2504,7 +2567,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="1" l="0.75000000000000011" r="0.75000000000000011" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75000000000000044" r="0.75000000000000044" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2530,7 +2593,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2BE14715-47DA-4F23-BAF5-24D2A024087A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2BE14715-47DA-4F23-BAF5-24D2A024087A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2568,7 +2631,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5E23D74E-C8F9-4086-8A84-7BF83C5152BB}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E23D74E-C8F9-4086-8A84-7BF83C5152BB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2606,7 +2669,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9ABF8EF7-8DD9-44DF-9280-7163A445B39C}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9ABF8EF7-8DD9-44DF-9280-7163A445B39C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2618,7 +2681,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -2638,7 +2701,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2709,7 +2772,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{60D52198-D506-4AA7-A57B-A8C3D0247DFE}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60D52198-D506-4AA7-A57B-A8C3D0247DFE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2721,7 +2784,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -2765,7 +2828,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{53DA16D2-291A-42A6-94EB-D697846FA36C}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53DA16D2-291A-42A6-94EB-D697846FA36C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2899,7 +2962,7 @@
         </a:effectLst>
         <a:extLst>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525" cmpd="sng">
+            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525" cmpd="sng">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -2949,7 +3012,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1C9D5358-04D5-45A9-9117-839674A38F39}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C9D5358-04D5-45A9-9117-839674A38F39}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2987,7 +3050,7 @@
         <xdr:cNvPr id="11" name="Picture 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C5460449-34D4-472A-97B4-74063FD93EF7}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5460449-34D4-472A-97B4-74063FD93EF7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2997,7 +3060,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3035,7 +3098,7 @@
         <xdr:cNvPr id="15" name="Picture 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B3257AE9-B407-40BD-AFE3-45B7CF3B360C}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3257AE9-B407-40BD-AFE3-45B7CF3B360C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3045,7 +3108,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3083,7 +3146,7 @@
         <xdr:cNvPr id="22" name="Picture 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BCA27E28-A006-440E-A37D-4323F3CD8901}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BCA27E28-A006-440E-A37D-4323F3CD8901}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3093,7 +3156,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3131,7 +3194,7 @@
         <xdr:cNvPr id="24" name="Picture 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B788E05D-6796-473C-B2C7-EEF8C7A50B05}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B788E05D-6796-473C-B2C7-EEF8C7A50B05}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3143,7 +3206,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3181,7 +3244,7 @@
         <xdr:cNvPr id="26" name="Picture 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F3A26610-B5E8-4FA3-BED3-4A266BF78BCD}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3A26610-B5E8-4FA3-BED3-4A266BF78BCD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3193,7 +3256,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3231,7 +3294,7 @@
         <xdr:cNvPr id="28" name="Picture 27">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A4521285-625F-4CA6-8FC5-4AFAFDF893A8}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4521285-625F-4CA6-8FC5-4AFAFDF893A8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3243,7 +3306,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3281,7 +3344,7 @@
         <xdr:cNvPr id="29" name="Picture 28">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{89936818-308B-4951-8C43-6322C73A3E3C}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89936818-308B-4951-8C43-6322C73A3E3C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3293,7 +3356,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3331,7 +3394,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B80C1EBE-F954-4FAF-9777-6966156D6D68}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B80C1EBE-F954-4FAF-9777-6966156D6D68}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3343,7 +3406,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3381,7 +3444,7 @@
         <xdr:cNvPr id="27" name="Picture 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DA25FA63-0A56-4155-9D0A-415548BF2225}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA25FA63-0A56-4155-9D0A-415548BF2225}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3393,7 +3456,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3426,7 +3489,7 @@
         <xdr:cNvPr id="30" name="Picture 29">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A407F95F-057E-476B-A252-51550475ED54}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A407F95F-057E-476B-A252-51550475ED54}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3438,7 +3501,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3471,7 +3534,7 @@
         <xdr:cNvPr id="31" name="Picture 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B1BA4C48-C2DC-4892-9738-3F8B87144095}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1BA4C48-C2DC-4892-9738-3F8B87144095}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3483,7 +3546,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3521,7 +3584,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{482A5AC2-E046-43EF-BB61-1DE7A7A1D4FB}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{482A5AC2-E046-43EF-BB61-1DE7A7A1D4FB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3533,7 +3596,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3566,7 +3629,7 @@
         <xdr:cNvPr id="35" name="Picture 34">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{63ADD56B-1BEA-4C18-896D-3A7E838FC08B}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63ADD56B-1BEA-4C18-896D-3A7E838FC08B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3578,7 +3641,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3890,7 +3953,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3900,7 +3963,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A5:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -3969,7 +4032,7 @@
       </c>
       <c r="C8" s="4">
         <f>'SMART- Export'!G8</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D8" s="4">
         <f>'SMART- Export'!G9</f>
@@ -3981,7 +4044,7 @@
       </c>
       <c r="F8" s="4">
         <f>SUM(B8:E8)</f>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G8" s="5">
         <f>(B8+C8+D8)/(F8)</f>
@@ -4007,7 +4070,7 @@
       </c>
       <c r="C10" s="7">
         <f>SUM(C8:C9)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D10" s="7">
         <f>SUM(D8:D9)</f>
@@ -4019,7 +4082,7 @@
       </c>
       <c r="F10" s="7">
         <f>SUM(F8:F9)</f>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G10" s="8">
         <f>SUM(G8:G8)</f>
@@ -4053,10 +4116,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.85546875" defaultRowHeight="15"/>
@@ -4219,7 +4282,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:4">
       <c r="A17" s="70"/>
       <c r="B17" s="10" t="s">
         <v>139</v>
@@ -4228,7 +4291,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:4">
       <c r="A18" s="70"/>
       <c r="B18" s="10" t="s">
         <v>140</v>
@@ -4237,7 +4300,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:4">
       <c r="A19" s="70"/>
       <c r="B19" s="10" t="s">
         <v>141</v>
@@ -4246,7 +4309,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:4">
       <c r="A20" s="70"/>
       <c r="B20" s="10" t="s">
         <v>142</v>
@@ -4255,7 +4318,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:4">
       <c r="A21" s="70"/>
       <c r="B21" s="10" t="s">
         <v>143</v>
@@ -4264,7 +4327,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:4">
       <c r="A22" s="70"/>
       <c r="B22" s="10" t="s">
         <v>144</v>
@@ -4273,7 +4336,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:4">
       <c r="A23" s="70"/>
       <c r="B23" s="10" t="s">
         <v>145</v>
@@ -4282,7 +4345,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:4">
       <c r="A24" s="70"/>
       <c r="B24" s="10" t="s">
         <v>146</v>
@@ -4291,13 +4354,13 @@
         <v>169</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:4">
       <c r="A25" s="70"/>
       <c r="C25" s="61" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:4">
       <c r="A26" s="70"/>
       <c r="B26" s="10" t="s">
         <v>156</v>
@@ -4306,66 +4369,99 @@
         <v>159</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:4">
       <c r="A27" s="70"/>
-    </row>
-    <row r="28" spans="1:3">
+      <c r="B27" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="C27" s="57" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" s="70"/>
-    </row>
-    <row r="29" spans="1:3">
+      <c r="C28" s="57"/>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29" s="70"/>
       <c r="B29" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
+        <v>211</v>
+      </c>
+      <c r="C29" s="57" t="s">
+        <v>209</v>
+      </c>
+      <c r="D29" s="57" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30" s="70"/>
       <c r="B30" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
+        <v>215</v>
+      </c>
+      <c r="C30" s="57" t="s">
+        <v>212</v>
+      </c>
+      <c r="D30" s="57" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31" s="70"/>
-      <c r="B31"/>
-    </row>
-    <row r="32" spans="1:3">
+      <c r="C31" s="57"/>
+      <c r="D31" s="57"/>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32" s="70"/>
-      <c r="B32"/>
-    </row>
-    <row r="33" spans="1:2">
+      <c r="B32" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33" s="70"/>
-      <c r="B33"/>
-    </row>
-    <row r="34" spans="1:2">
+      <c r="C33" s="10" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
       <c r="A34" s="70"/>
-    </row>
-    <row r="35" spans="1:2">
+      <c r="B34"/>
+    </row>
+    <row r="35" spans="1:3">
       <c r="A35" s="70"/>
-    </row>
-    <row r="36" spans="1:2">
+      <c r="B35"/>
+    </row>
+    <row r="36" spans="1:3">
       <c r="A36" s="70"/>
-    </row>
-    <row r="37" spans="1:2">
+      <c r="B36"/>
+    </row>
+    <row r="37" spans="1:3">
       <c r="A37" s="70"/>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:3">
       <c r="A38" s="70"/>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:3">
       <c r="A39" s="70"/>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:3">
       <c r="A40" s="70"/>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="70"/>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="70"/>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="70"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A2:A40"/>
+    <mergeCell ref="A2:A43"/>
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4376,10 +4472,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I886"/>
+  <dimension ref="A1:I884"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -5119,7 +5215,7 @@
         <v>44</v>
       </c>
       <c r="C7" s="23">
-        <v>43780</v>
+        <v>43999</v>
       </c>
       <c r="D7" s="16"/>
       <c r="E7" s="13"/>
@@ -5127,7 +5223,7 @@
         <v>4</v>
       </c>
       <c r="G7" s="25">
-        <f>COUNTIF(G11:G1012,"Pass")</f>
+        <f>COUNTIF(G11:G1010,"Pass")</f>
         <v>21</v>
       </c>
     </row>
@@ -5143,8 +5239,8 @@
         <v>5</v>
       </c>
       <c r="G8" s="25">
-        <f>COUNTIF(G12:G1013,"Fail")</f>
-        <v>2</v>
+        <f>COUNTIF(G12:G1011,"Fail")</f>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.75" thickBot="1">
@@ -5161,7 +5257,7 @@
         <v>6</v>
       </c>
       <c r="G9" s="25">
-        <f>COUNTIF(G13:G1014,"Blocked")</f>
+        <f>COUNTIF(G13:G1012,"Blocked")</f>
         <v>1</v>
       </c>
     </row>
@@ -5177,7 +5273,7 @@
         <v>7</v>
       </c>
       <c r="G10" s="25">
-        <f>COUNTIF(G14:G1015,"Not Executed")</f>
+        <f>COUNTIF(G14:G1013,"Not Executed")</f>
         <v>0</v>
       </c>
     </row>
@@ -5202,7 +5298,7 @@
       </c>
       <c r="C12" s="15">
         <f>G8</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D12" s="16"/>
       <c r="E12" s="13"/>
@@ -5271,12 +5367,12 @@
       <c r="A18" s="40" t="s">
         <v>78</v>
       </c>
-      <c r="B18" s="71" t="s">
+      <c r="B18" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="72"/>
-      <c r="D18" s="72"/>
-      <c r="E18" s="73"/>
+      <c r="C18" s="75"/>
+      <c r="D18" s="75"/>
+      <c r="E18" s="76"/>
       <c r="F18" s="41" t="s">
         <v>54</v>
       </c>
@@ -5293,14 +5389,14 @@
       <c r="A19" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="B19" s="74" t="s">
+      <c r="B19" s="77" t="s">
         <v>57</v>
       </c>
-      <c r="C19" s="75"/>
-      <c r="D19" s="75"/>
-      <c r="E19" s="75"/>
-      <c r="F19" s="75"/>
-      <c r="G19" s="76"/>
+      <c r="C19" s="78"/>
+      <c r="D19" s="78"/>
+      <c r="E19" s="78"/>
+      <c r="F19" s="78"/>
+      <c r="G19" s="79"/>
       <c r="I19"/>
     </row>
     <row r="20" spans="1:9" s="38" customFormat="1">
@@ -5347,23 +5443,23 @@
       <c r="A22" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="B22" s="77"/>
-      <c r="C22" s="78"/>
-      <c r="D22" s="78"/>
-      <c r="E22" s="78"/>
-      <c r="F22" s="78"/>
-      <c r="G22" s="79"/>
+      <c r="B22" s="71"/>
+      <c r="C22" s="72"/>
+      <c r="D22" s="72"/>
+      <c r="E22" s="72"/>
+      <c r="F22" s="72"/>
+      <c r="G22" s="73"/>
     </row>
     <row r="23" spans="1:9" s="38" customFormat="1">
       <c r="A23" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="B23" s="71" t="s">
+      <c r="B23" s="74" t="s">
         <v>122</v>
       </c>
-      <c r="C23" s="72"/>
-      <c r="D23" s="72"/>
-      <c r="E23" s="73"/>
+      <c r="C23" s="75"/>
+      <c r="D23" s="75"/>
+      <c r="E23" s="76"/>
       <c r="F23" s="41" t="s">
         <v>54</v>
       </c>
@@ -5376,14 +5472,14 @@
       <c r="A24" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="B24" s="74" t="s">
+      <c r="B24" s="77" t="s">
         <v>57</v>
       </c>
-      <c r="C24" s="75"/>
-      <c r="D24" s="75"/>
-      <c r="E24" s="75"/>
-      <c r="F24" s="75"/>
-      <c r="G24" s="76"/>
+      <c r="C24" s="78"/>
+      <c r="D24" s="78"/>
+      <c r="E24" s="78"/>
+      <c r="F24" s="78"/>
+      <c r="G24" s="79"/>
     </row>
     <row r="25" spans="1:9" s="38" customFormat="1">
       <c r="A25" s="44" t="s">
@@ -5463,23 +5559,23 @@
       <c r="A29" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="B29" s="77"/>
-      <c r="C29" s="78"/>
-      <c r="D29" s="78"/>
-      <c r="E29" s="78"/>
-      <c r="F29" s="78"/>
-      <c r="G29" s="79"/>
+      <c r="B29" s="71"/>
+      <c r="C29" s="72"/>
+      <c r="D29" s="72"/>
+      <c r="E29" s="72"/>
+      <c r="F29" s="72"/>
+      <c r="G29" s="73"/>
     </row>
     <row r="30" spans="1:9" s="38" customFormat="1">
       <c r="A30" s="40" t="s">
         <v>80</v>
       </c>
-      <c r="B30" s="71" t="s">
+      <c r="B30" s="74" t="s">
         <v>109</v>
       </c>
-      <c r="C30" s="72"/>
-      <c r="D30" s="72"/>
-      <c r="E30" s="73"/>
+      <c r="C30" s="75"/>
+      <c r="D30" s="75"/>
+      <c r="E30" s="76"/>
       <c r="F30" s="41" t="s">
         <v>54</v>
       </c>
@@ -5492,14 +5588,14 @@
       <c r="A31" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="B31" s="74" t="s">
+      <c r="B31" s="77" t="s">
         <v>57</v>
       </c>
-      <c r="C31" s="75"/>
-      <c r="D31" s="75"/>
-      <c r="E31" s="75"/>
-      <c r="F31" s="75"/>
-      <c r="G31" s="76"/>
+      <c r="C31" s="78"/>
+      <c r="D31" s="78"/>
+      <c r="E31" s="78"/>
+      <c r="F31" s="78"/>
+      <c r="G31" s="79"/>
     </row>
     <row r="32" spans="1:9" s="38" customFormat="1">
       <c r="A32" s="44" t="s">
@@ -5579,23 +5675,23 @@
       <c r="A36" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="B36" s="77"/>
-      <c r="C36" s="78"/>
-      <c r="D36" s="78"/>
-      <c r="E36" s="78"/>
-      <c r="F36" s="78"/>
-      <c r="G36" s="79"/>
+      <c r="B36" s="71"/>
+      <c r="C36" s="72"/>
+      <c r="D36" s="72"/>
+      <c r="E36" s="72"/>
+      <c r="F36" s="72"/>
+      <c r="G36" s="73"/>
     </row>
     <row r="37" spans="1:7" s="38" customFormat="1">
       <c r="A37" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="B37" s="71" t="s">
+      <c r="B37" s="74" t="s">
         <v>112</v>
       </c>
-      <c r="C37" s="72"/>
-      <c r="D37" s="72"/>
-      <c r="E37" s="73"/>
+      <c r="C37" s="75"/>
+      <c r="D37" s="75"/>
+      <c r="E37" s="76"/>
       <c r="F37" s="41" t="s">
         <v>54</v>
       </c>
@@ -5608,14 +5704,14 @@
       <c r="A38" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="B38" s="74" t="s">
+      <c r="B38" s="77" t="s">
         <v>57</v>
       </c>
-      <c r="C38" s="75"/>
-      <c r="D38" s="75"/>
-      <c r="E38" s="75"/>
-      <c r="F38" s="75"/>
-      <c r="G38" s="76"/>
+      <c r="C38" s="78"/>
+      <c r="D38" s="78"/>
+      <c r="E38" s="78"/>
+      <c r="F38" s="78"/>
+      <c r="G38" s="79"/>
     </row>
     <row r="39" spans="1:7" s="38" customFormat="1">
       <c r="A39" s="44" t="s">
@@ -5695,23 +5791,23 @@
       <c r="A43" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="B43" s="77"/>
-      <c r="C43" s="78"/>
-      <c r="D43" s="78"/>
-      <c r="E43" s="78"/>
-      <c r="F43" s="78"/>
-      <c r="G43" s="79"/>
+      <c r="B43" s="71"/>
+      <c r="C43" s="72"/>
+      <c r="D43" s="72"/>
+      <c r="E43" s="72"/>
+      <c r="F43" s="72"/>
+      <c r="G43" s="73"/>
     </row>
     <row r="44" spans="1:7" s="38" customFormat="1">
       <c r="A44" s="40" t="s">
         <v>82</v>
       </c>
-      <c r="B44" s="71" t="s">
+      <c r="B44" s="74" t="s">
         <v>115</v>
       </c>
-      <c r="C44" s="72"/>
-      <c r="D44" s="72"/>
-      <c r="E44" s="73"/>
+      <c r="C44" s="75"/>
+      <c r="D44" s="75"/>
+      <c r="E44" s="76"/>
       <c r="F44" s="41" t="s">
         <v>54</v>
       </c>
@@ -5724,14 +5820,14 @@
       <c r="A45" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="B45" s="74" t="s">
+      <c r="B45" s="77" t="s">
         <v>57</v>
       </c>
-      <c r="C45" s="75"/>
-      <c r="D45" s="75"/>
-      <c r="E45" s="75"/>
-      <c r="F45" s="75"/>
-      <c r="G45" s="76"/>
+      <c r="C45" s="78"/>
+      <c r="D45" s="78"/>
+      <c r="E45" s="78"/>
+      <c r="F45" s="78"/>
+      <c r="G45" s="79"/>
     </row>
     <row r="46" spans="1:7" s="38" customFormat="1">
       <c r="A46" s="44" t="s">
@@ -5794,23 +5890,23 @@
       <c r="A49" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="B49" s="77"/>
-      <c r="C49" s="78"/>
-      <c r="D49" s="78"/>
-      <c r="E49" s="78"/>
-      <c r="F49" s="78"/>
-      <c r="G49" s="79"/>
+      <c r="B49" s="71"/>
+      <c r="C49" s="72"/>
+      <c r="D49" s="72"/>
+      <c r="E49" s="72"/>
+      <c r="F49" s="72"/>
+      <c r="G49" s="73"/>
     </row>
     <row r="50" spans="1:9" s="38" customFormat="1">
       <c r="A50" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="B50" s="71" t="s">
+      <c r="B50" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="C50" s="72"/>
-      <c r="D50" s="72"/>
-      <c r="E50" s="73"/>
+      <c r="C50" s="75"/>
+      <c r="D50" s="75"/>
+      <c r="E50" s="76"/>
       <c r="F50" s="41" t="s">
         <v>54</v>
       </c>
@@ -5823,14 +5919,14 @@
       <c r="A51" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="B51" s="74" t="s">
+      <c r="B51" s="77" t="s">
         <v>57</v>
       </c>
-      <c r="C51" s="75"/>
-      <c r="D51" s="75"/>
-      <c r="E51" s="75"/>
-      <c r="F51" s="75"/>
-      <c r="G51" s="76"/>
+      <c r="C51" s="78"/>
+      <c r="D51" s="78"/>
+      <c r="E51" s="78"/>
+      <c r="F51" s="78"/>
+      <c r="G51" s="79"/>
     </row>
     <row r="52" spans="1:9" s="38" customFormat="1">
       <c r="A52" s="44" t="s">
@@ -5910,23 +6006,23 @@
       <c r="A56" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="B56" s="77"/>
-      <c r="C56" s="78"/>
-      <c r="D56" s="78"/>
-      <c r="E56" s="78"/>
-      <c r="F56" s="78"/>
-      <c r="G56" s="79"/>
+      <c r="B56" s="71"/>
+      <c r="C56" s="72"/>
+      <c r="D56" s="72"/>
+      <c r="E56" s="72"/>
+      <c r="F56" s="72"/>
+      <c r="G56" s="73"/>
     </row>
     <row r="57" spans="1:9" s="38" customFormat="1">
       <c r="A57" s="40" t="s">
         <v>84</v>
       </c>
-      <c r="B57" s="71" t="s">
+      <c r="B57" s="74" t="s">
         <v>121</v>
       </c>
-      <c r="C57" s="72"/>
-      <c r="D57" s="72"/>
-      <c r="E57" s="73"/>
+      <c r="C57" s="75"/>
+      <c r="D57" s="75"/>
+      <c r="E57" s="76"/>
       <c r="F57" s="41" t="s">
         <v>54</v>
       </c>
@@ -5939,14 +6035,14 @@
       <c r="A58" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="B58" s="74" t="s">
+      <c r="B58" s="77" t="s">
         <v>57</v>
       </c>
-      <c r="C58" s="75"/>
-      <c r="D58" s="75"/>
-      <c r="E58" s="75"/>
-      <c r="F58" s="75"/>
-      <c r="G58" s="76"/>
+      <c r="C58" s="78"/>
+      <c r="D58" s="78"/>
+      <c r="E58" s="78"/>
+      <c r="F58" s="78"/>
+      <c r="G58" s="79"/>
     </row>
     <row r="59" spans="1:9" s="38" customFormat="1">
       <c r="A59" s="44" t="s">
@@ -6029,23 +6125,23 @@
       <c r="A63" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="B63" s="77"/>
-      <c r="C63" s="78"/>
-      <c r="D63" s="78"/>
-      <c r="E63" s="78"/>
-      <c r="F63" s="78"/>
-      <c r="G63" s="79"/>
+      <c r="B63" s="71"/>
+      <c r="C63" s="72"/>
+      <c r="D63" s="72"/>
+      <c r="E63" s="72"/>
+      <c r="F63" s="72"/>
+      <c r="G63" s="73"/>
     </row>
     <row r="64" spans="1:9" s="38" customFormat="1">
       <c r="A64" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="B64" s="71" t="s">
+      <c r="B64" s="74" t="s">
         <v>124</v>
       </c>
-      <c r="C64" s="72"/>
-      <c r="D64" s="72"/>
-      <c r="E64" s="73"/>
+      <c r="C64" s="75"/>
+      <c r="D64" s="75"/>
+      <c r="E64" s="76"/>
       <c r="F64" s="41" t="s">
         <v>54</v>
       </c>
@@ -6058,14 +6154,14 @@
       <c r="A65" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="B65" s="74" t="s">
+      <c r="B65" s="77" t="s">
         <v>57</v>
       </c>
-      <c r="C65" s="75"/>
-      <c r="D65" s="75"/>
-      <c r="E65" s="75"/>
-      <c r="F65" s="75"/>
-      <c r="G65" s="76"/>
+      <c r="C65" s="78"/>
+      <c r="D65" s="78"/>
+      <c r="E65" s="78"/>
+      <c r="F65" s="78"/>
+      <c r="G65" s="79"/>
     </row>
     <row r="66" spans="1:7" s="38" customFormat="1">
       <c r="A66" s="44" t="s">
@@ -6162,23 +6258,23 @@
       <c r="A71" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="B71" s="77"/>
-      <c r="C71" s="78"/>
-      <c r="D71" s="78"/>
-      <c r="E71" s="78"/>
-      <c r="F71" s="78"/>
-      <c r="G71" s="79"/>
+      <c r="B71" s="71"/>
+      <c r="C71" s="72"/>
+      <c r="D71" s="72"/>
+      <c r="E71" s="72"/>
+      <c r="F71" s="72"/>
+      <c r="G71" s="73"/>
     </row>
     <row r="72" spans="1:7" s="38" customFormat="1">
       <c r="A72" s="40" t="s">
         <v>127</v>
       </c>
-      <c r="B72" s="71" t="s">
+      <c r="B72" s="74" t="s">
         <v>128</v>
       </c>
-      <c r="C72" s="72"/>
-      <c r="D72" s="72"/>
-      <c r="E72" s="73"/>
+      <c r="C72" s="75"/>
+      <c r="D72" s="75"/>
+      <c r="E72" s="76"/>
       <c r="F72" s="41" t="s">
         <v>54</v>
       </c>
@@ -6191,14 +6287,14 @@
       <c r="A73" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="B73" s="74" t="s">
+      <c r="B73" s="77" t="s">
         <v>57</v>
       </c>
-      <c r="C73" s="75"/>
-      <c r="D73" s="75"/>
-      <c r="E73" s="75"/>
-      <c r="F73" s="75"/>
-      <c r="G73" s="76"/>
+      <c r="C73" s="78"/>
+      <c r="D73" s="78"/>
+      <c r="E73" s="78"/>
+      <c r="F73" s="78"/>
+      <c r="G73" s="79"/>
     </row>
     <row r="74" spans="1:7" s="38" customFormat="1">
       <c r="A74" s="44" t="s">
@@ -6295,23 +6391,23 @@
       <c r="A79" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="B79" s="77"/>
-      <c r="C79" s="78"/>
-      <c r="D79" s="78"/>
-      <c r="E79" s="78"/>
-      <c r="F79" s="78"/>
-      <c r="G79" s="79"/>
+      <c r="B79" s="71"/>
+      <c r="C79" s="72"/>
+      <c r="D79" s="72"/>
+      <c r="E79" s="72"/>
+      <c r="F79" s="72"/>
+      <c r="G79" s="73"/>
     </row>
     <row r="80" spans="1:7">
       <c r="A80" s="40" t="s">
         <v>129</v>
       </c>
-      <c r="B80" s="71" t="s">
+      <c r="B80" s="74" t="s">
         <v>130</v>
       </c>
-      <c r="C80" s="72"/>
-      <c r="D80" s="72"/>
-      <c r="E80" s="73"/>
+      <c r="C80" s="75"/>
+      <c r="D80" s="75"/>
+      <c r="E80" s="76"/>
       <c r="F80" s="41" t="s">
         <v>54</v>
       </c>
@@ -6324,14 +6420,14 @@
       <c r="A81" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="B81" s="74" t="s">
+      <c r="B81" s="77" t="s">
         <v>71</v>
       </c>
-      <c r="C81" s="75"/>
-      <c r="D81" s="75"/>
-      <c r="E81" s="75"/>
-      <c r="F81" s="75"/>
-      <c r="G81" s="76"/>
+      <c r="C81" s="78"/>
+      <c r="D81" s="78"/>
+      <c r="E81" s="78"/>
+      <c r="F81" s="78"/>
+      <c r="G81" s="79"/>
     </row>
     <row r="82" spans="1:7">
       <c r="A82" s="44" t="s">
@@ -6428,23 +6524,23 @@
       <c r="A87" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="B87" s="77"/>
-      <c r="C87" s="78"/>
-      <c r="D87" s="78"/>
-      <c r="E87" s="78"/>
-      <c r="F87" s="78"/>
-      <c r="G87" s="79"/>
+      <c r="B87" s="71"/>
+      <c r="C87" s="72"/>
+      <c r="D87" s="72"/>
+      <c r="E87" s="72"/>
+      <c r="F87" s="72"/>
+      <c r="G87" s="73"/>
     </row>
     <row r="88" spans="1:7">
       <c r="A88" s="40" t="s">
         <v>135</v>
       </c>
-      <c r="B88" s="71" t="s">
+      <c r="B88" s="74" t="s">
         <v>88</v>
       </c>
-      <c r="C88" s="72"/>
-      <c r="D88" s="72"/>
-      <c r="E88" s="73"/>
+      <c r="C88" s="75"/>
+      <c r="D88" s="75"/>
+      <c r="E88" s="76"/>
       <c r="F88" s="41" t="s">
         <v>54</v>
       </c>
@@ -6457,14 +6553,14 @@
       <c r="A89" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="B89" s="74" t="s">
+      <c r="B89" s="77" t="s">
         <v>71</v>
       </c>
-      <c r="C89" s="75"/>
-      <c r="D89" s="75"/>
-      <c r="E89" s="75"/>
-      <c r="F89" s="75"/>
-      <c r="G89" s="76"/>
+      <c r="C89" s="78"/>
+      <c r="D89" s="78"/>
+      <c r="E89" s="78"/>
+      <c r="F89" s="78"/>
+      <c r="G89" s="79"/>
     </row>
     <row r="90" spans="1:7">
       <c r="A90" s="44" t="s">
@@ -6561,23 +6657,23 @@
       <c r="A95" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="B95" s="77"/>
-      <c r="C95" s="78"/>
-      <c r="D95" s="78"/>
-      <c r="E95" s="78"/>
-      <c r="F95" s="78"/>
-      <c r="G95" s="79"/>
+      <c r="B95" s="71"/>
+      <c r="C95" s="72"/>
+      <c r="D95" s="72"/>
+      <c r="E95" s="72"/>
+      <c r="F95" s="72"/>
+      <c r="G95" s="73"/>
     </row>
     <row r="96" spans="1:7">
       <c r="A96" s="40" t="s">
         <v>86</v>
       </c>
-      <c r="B96" s="71" t="s">
+      <c r="B96" s="74" t="s">
         <v>101</v>
       </c>
-      <c r="C96" s="72"/>
-      <c r="D96" s="72"/>
-      <c r="E96" s="73"/>
+      <c r="C96" s="75"/>
+      <c r="D96" s="75"/>
+      <c r="E96" s="76"/>
       <c r="F96" s="41" t="s">
         <v>54</v>
       </c>
@@ -6590,14 +6686,14 @@
       <c r="A97" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="B97" s="74" t="s">
+      <c r="B97" s="77" t="s">
         <v>71</v>
       </c>
-      <c r="C97" s="75"/>
-      <c r="D97" s="75"/>
-      <c r="E97" s="75"/>
-      <c r="F97" s="75"/>
-      <c r="G97" s="76"/>
+      <c r="C97" s="78"/>
+      <c r="D97" s="78"/>
+      <c r="E97" s="78"/>
+      <c r="F97" s="78"/>
+      <c r="G97" s="79"/>
     </row>
     <row r="98" spans="1:7">
       <c r="A98" s="44" t="s">
@@ -6694,23 +6790,23 @@
       <c r="A103" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="B103" s="77"/>
-      <c r="C103" s="78"/>
-      <c r="D103" s="78"/>
-      <c r="E103" s="78"/>
-      <c r="F103" s="78"/>
-      <c r="G103" s="79"/>
+      <c r="B103" s="71"/>
+      <c r="C103" s="72"/>
+      <c r="D103" s="72"/>
+      <c r="E103" s="72"/>
+      <c r="F103" s="72"/>
+      <c r="G103" s="73"/>
     </row>
     <row r="104" spans="1:7">
       <c r="A104" s="40" t="s">
         <v>87</v>
       </c>
-      <c r="B104" s="71" t="s">
+      <c r="B104" s="74" t="s">
         <v>29</v>
       </c>
-      <c r="C104" s="72"/>
-      <c r="D104" s="72"/>
-      <c r="E104" s="73"/>
+      <c r="C104" s="75"/>
+      <c r="D104" s="75"/>
+      <c r="E104" s="76"/>
       <c r="F104" s="41" t="s">
         <v>54</v>
       </c>
@@ -6723,14 +6819,14 @@
       <c r="A105" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="B105" s="74" t="s">
+      <c r="B105" s="77" t="s">
         <v>71</v>
       </c>
-      <c r="C105" s="75"/>
-      <c r="D105" s="75"/>
-      <c r="E105" s="75"/>
-      <c r="F105" s="75"/>
-      <c r="G105" s="76"/>
+      <c r="C105" s="78"/>
+      <c r="D105" s="78"/>
+      <c r="E105" s="78"/>
+      <c r="F105" s="78"/>
+      <c r="G105" s="79"/>
     </row>
     <row r="106" spans="1:7">
       <c r="A106" s="44" t="s">
@@ -6827,23 +6923,23 @@
       <c r="A111" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="B111" s="77"/>
-      <c r="C111" s="78"/>
-      <c r="D111" s="78"/>
-      <c r="E111" s="78"/>
-      <c r="F111" s="78"/>
-      <c r="G111" s="79"/>
+      <c r="B111" s="71"/>
+      <c r="C111" s="72"/>
+      <c r="D111" s="72"/>
+      <c r="E111" s="72"/>
+      <c r="F111" s="72"/>
+      <c r="G111" s="73"/>
     </row>
     <row r="112" spans="1:7">
       <c r="A112" s="40" t="s">
         <v>160</v>
       </c>
-      <c r="B112" s="71" t="s">
+      <c r="B112" s="74" t="s">
         <v>161</v>
       </c>
-      <c r="C112" s="72"/>
-      <c r="D112" s="72"/>
-      <c r="E112" s="73"/>
+      <c r="C112" s="75"/>
+      <c r="D112" s="75"/>
+      <c r="E112" s="76"/>
       <c r="F112" s="41" t="s">
         <v>54</v>
       </c>
@@ -6856,14 +6952,14 @@
       <c r="A113" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="B113" s="74" t="s">
+      <c r="B113" s="77" t="s">
         <v>71</v>
       </c>
-      <c r="C113" s="75"/>
-      <c r="D113" s="75"/>
-      <c r="E113" s="75"/>
-      <c r="F113" s="75"/>
-      <c r="G113" s="76"/>
+      <c r="C113" s="78"/>
+      <c r="D113" s="78"/>
+      <c r="E113" s="78"/>
+      <c r="F113" s="78"/>
+      <c r="G113" s="79"/>
     </row>
     <row r="114" spans="1:7">
       <c r="A114" s="44" t="s">
@@ -6926,23 +7022,23 @@
       <c r="A117" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="B117" s="77"/>
-      <c r="C117" s="78"/>
-      <c r="D117" s="78"/>
-      <c r="E117" s="78"/>
-      <c r="F117" s="78"/>
-      <c r="G117" s="79"/>
+      <c r="B117" s="71"/>
+      <c r="C117" s="72"/>
+      <c r="D117" s="72"/>
+      <c r="E117" s="72"/>
+      <c r="F117" s="72"/>
+      <c r="G117" s="73"/>
     </row>
     <row r="118" spans="1:7">
       <c r="A118" s="40" t="s">
         <v>163</v>
       </c>
-      <c r="B118" s="71" t="s">
+      <c r="B118" s="74" t="s">
         <v>147</v>
       </c>
-      <c r="C118" s="72"/>
-      <c r="D118" s="72"/>
-      <c r="E118" s="73"/>
+      <c r="C118" s="75"/>
+      <c r="D118" s="75"/>
+      <c r="E118" s="76"/>
       <c r="F118" s="41" t="s">
         <v>54</v>
       </c>
@@ -6955,14 +7051,14 @@
       <c r="A119" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="B119" s="74" t="s">
+      <c r="B119" s="77" t="s">
         <v>71</v>
       </c>
-      <c r="C119" s="75"/>
-      <c r="D119" s="75"/>
-      <c r="E119" s="75"/>
-      <c r="F119" s="75"/>
-      <c r="G119" s="76"/>
+      <c r="C119" s="78"/>
+      <c r="D119" s="78"/>
+      <c r="E119" s="78"/>
+      <c r="F119" s="78"/>
+      <c r="G119" s="79"/>
     </row>
     <row r="120" spans="1:7">
       <c r="A120" s="44" t="s">
@@ -7042,23 +7138,23 @@
       <c r="A124" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="B124" s="77"/>
-      <c r="C124" s="78"/>
-      <c r="D124" s="78"/>
-      <c r="E124" s="78"/>
-      <c r="F124" s="78"/>
-      <c r="G124" s="79"/>
+      <c r="B124" s="71"/>
+      <c r="C124" s="72"/>
+      <c r="D124" s="72"/>
+      <c r="E124" s="72"/>
+      <c r="F124" s="72"/>
+      <c r="G124" s="73"/>
     </row>
     <row r="125" spans="1:7">
       <c r="A125" s="40" t="s">
         <v>166</v>
       </c>
-      <c r="B125" s="71" t="s">
+      <c r="B125" s="74" t="s">
         <v>148</v>
       </c>
-      <c r="C125" s="72"/>
-      <c r="D125" s="72"/>
-      <c r="E125" s="73"/>
+      <c r="C125" s="75"/>
+      <c r="D125" s="75"/>
+      <c r="E125" s="76"/>
       <c r="F125" s="41" t="s">
         <v>54</v>
       </c>
@@ -7071,14 +7167,14 @@
       <c r="A126" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="B126" s="74" t="s">
+      <c r="B126" s="77" t="s">
         <v>71</v>
       </c>
-      <c r="C126" s="75"/>
-      <c r="D126" s="75"/>
-      <c r="E126" s="75"/>
-      <c r="F126" s="75"/>
-      <c r="G126" s="76"/>
+      <c r="C126" s="78"/>
+      <c r="D126" s="78"/>
+      <c r="E126" s="78"/>
+      <c r="F126" s="78"/>
+      <c r="G126" s="79"/>
     </row>
     <row r="127" spans="1:7">
       <c r="A127" s="44" t="s">
@@ -7175,23 +7271,23 @@
       <c r="A132" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="B132" s="77"/>
-      <c r="C132" s="78"/>
-      <c r="D132" s="78"/>
-      <c r="E132" s="78"/>
-      <c r="F132" s="78"/>
-      <c r="G132" s="79"/>
+      <c r="B132" s="71"/>
+      <c r="C132" s="72"/>
+      <c r="D132" s="72"/>
+      <c r="E132" s="72"/>
+      <c r="F132" s="72"/>
+      <c r="G132" s="73"/>
     </row>
     <row r="133" spans="1:7">
       <c r="A133" s="40" t="s">
         <v>170</v>
       </c>
-      <c r="B133" s="71" t="s">
+      <c r="B133" s="74" t="s">
         <v>150</v>
       </c>
-      <c r="C133" s="72"/>
-      <c r="D133" s="72"/>
-      <c r="E133" s="73"/>
+      <c r="C133" s="75"/>
+      <c r="D133" s="75"/>
+      <c r="E133" s="76"/>
       <c r="F133" s="41" t="s">
         <v>54</v>
       </c>
@@ -7204,14 +7300,14 @@
       <c r="A134" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="B134" s="74" t="s">
+      <c r="B134" s="77" t="s">
         <v>71</v>
       </c>
-      <c r="C134" s="75"/>
-      <c r="D134" s="75"/>
-      <c r="E134" s="75"/>
-      <c r="F134" s="75"/>
-      <c r="G134" s="76"/>
+      <c r="C134" s="78"/>
+      <c r="D134" s="78"/>
+      <c r="E134" s="78"/>
+      <c r="F134" s="78"/>
+      <c r="G134" s="79"/>
     </row>
     <row r="135" spans="1:7">
       <c r="A135" s="44" t="s">
@@ -7308,23 +7404,23 @@
       <c r="A140" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="B140" s="77"/>
-      <c r="C140" s="78"/>
-      <c r="D140" s="78"/>
-      <c r="E140" s="78"/>
-      <c r="F140" s="78"/>
-      <c r="G140" s="79"/>
+      <c r="B140" s="71"/>
+      <c r="C140" s="72"/>
+      <c r="D140" s="72"/>
+      <c r="E140" s="72"/>
+      <c r="F140" s="72"/>
+      <c r="G140" s="73"/>
     </row>
     <row r="141" spans="1:7">
       <c r="A141" s="40" t="s">
         <v>173</v>
       </c>
-      <c r="B141" s="71" t="s">
+      <c r="B141" s="74" t="s">
         <v>149</v>
       </c>
-      <c r="C141" s="72"/>
-      <c r="D141" s="72"/>
-      <c r="E141" s="73"/>
+      <c r="C141" s="75"/>
+      <c r="D141" s="75"/>
+      <c r="E141" s="76"/>
       <c r="F141" s="41" t="s">
         <v>54</v>
       </c>
@@ -7337,14 +7433,14 @@
       <c r="A142" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="B142" s="74" t="s">
+      <c r="B142" s="77" t="s">
         <v>71</v>
       </c>
-      <c r="C142" s="75"/>
-      <c r="D142" s="75"/>
-      <c r="E142" s="75"/>
-      <c r="F142" s="75"/>
-      <c r="G142" s="76"/>
+      <c r="C142" s="78"/>
+      <c r="D142" s="78"/>
+      <c r="E142" s="78"/>
+      <c r="F142" s="78"/>
+      <c r="G142" s="79"/>
     </row>
     <row r="143" spans="1:7">
       <c r="A143" s="44" t="s">
@@ -7441,23 +7537,23 @@
       <c r="A148" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="B148" s="77"/>
-      <c r="C148" s="78"/>
-      <c r="D148" s="78"/>
-      <c r="E148" s="78"/>
-      <c r="F148" s="78"/>
-      <c r="G148" s="79"/>
+      <c r="B148" s="71"/>
+      <c r="C148" s="72"/>
+      <c r="D148" s="72"/>
+      <c r="E148" s="72"/>
+      <c r="F148" s="72"/>
+      <c r="G148" s="73"/>
     </row>
     <row r="149" spans="1:7">
       <c r="A149" s="40" t="s">
         <v>176</v>
       </c>
-      <c r="B149" s="71" t="s">
+      <c r="B149" s="74" t="s">
         <v>151</v>
       </c>
-      <c r="C149" s="72"/>
-      <c r="D149" s="72"/>
-      <c r="E149" s="73"/>
+      <c r="C149" s="75"/>
+      <c r="D149" s="75"/>
+      <c r="E149" s="76"/>
       <c r="F149" s="41" t="s">
         <v>54</v>
       </c>
@@ -7470,14 +7566,14 @@
       <c r="A150" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="B150" s="74" t="s">
+      <c r="B150" s="77" t="s">
         <v>71</v>
       </c>
-      <c r="C150" s="75"/>
-      <c r="D150" s="75"/>
-      <c r="E150" s="75"/>
-      <c r="F150" s="75"/>
-      <c r="G150" s="76"/>
+      <c r="C150" s="78"/>
+      <c r="D150" s="78"/>
+      <c r="E150" s="78"/>
+      <c r="F150" s="78"/>
+      <c r="G150" s="79"/>
     </row>
     <row r="151" spans="1:7">
       <c r="A151" s="44" t="s">
@@ -7574,23 +7670,23 @@
       <c r="A156" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="B156" s="77"/>
-      <c r="C156" s="78"/>
-      <c r="D156" s="78"/>
-      <c r="E156" s="78"/>
-      <c r="F156" s="78"/>
-      <c r="G156" s="79"/>
+      <c r="B156" s="71"/>
+      <c r="C156" s="72"/>
+      <c r="D156" s="72"/>
+      <c r="E156" s="72"/>
+      <c r="F156" s="72"/>
+      <c r="G156" s="73"/>
     </row>
     <row r="157" spans="1:7">
       <c r="A157" s="40" t="s">
         <v>179</v>
       </c>
-      <c r="B157" s="71" t="s">
+      <c r="B157" s="74" t="s">
         <v>152</v>
       </c>
-      <c r="C157" s="72"/>
-      <c r="D157" s="72"/>
-      <c r="E157" s="73"/>
+      <c r="C157" s="75"/>
+      <c r="D157" s="75"/>
+      <c r="E157" s="76"/>
       <c r="F157" s="41" t="s">
         <v>54</v>
       </c>
@@ -7603,14 +7699,14 @@
       <c r="A158" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="B158" s="74" t="s">
+      <c r="B158" s="77" t="s">
         <v>71</v>
       </c>
-      <c r="C158" s="75"/>
-      <c r="D158" s="75"/>
-      <c r="E158" s="75"/>
-      <c r="F158" s="75"/>
-      <c r="G158" s="76"/>
+      <c r="C158" s="78"/>
+      <c r="D158" s="78"/>
+      <c r="E158" s="78"/>
+      <c r="F158" s="78"/>
+      <c r="G158" s="79"/>
     </row>
     <row r="159" spans="1:7">
       <c r="A159" s="44" t="s">
@@ -7724,23 +7820,23 @@
       <c r="A165" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="B165" s="77"/>
-      <c r="C165" s="78"/>
-      <c r="D165" s="78"/>
-      <c r="E165" s="78"/>
-      <c r="F165" s="78"/>
-      <c r="G165" s="79"/>
+      <c r="B165" s="71"/>
+      <c r="C165" s="72"/>
+      <c r="D165" s="72"/>
+      <c r="E165" s="72"/>
+      <c r="F165" s="72"/>
+      <c r="G165" s="73"/>
     </row>
     <row r="166" spans="1:7">
       <c r="A166" s="40" t="s">
         <v>182</v>
       </c>
-      <c r="B166" s="71" t="s">
+      <c r="B166" s="74" t="s">
         <v>153</v>
       </c>
-      <c r="C166" s="72"/>
-      <c r="D166" s="72"/>
-      <c r="E166" s="73"/>
+      <c r="C166" s="75"/>
+      <c r="D166" s="75"/>
+      <c r="E166" s="76"/>
       <c r="F166" s="41" t="s">
         <v>54</v>
       </c>
@@ -7753,14 +7849,14 @@
       <c r="A167" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="B167" s="74" t="s">
+      <c r="B167" s="77" t="s">
         <v>71</v>
       </c>
-      <c r="C167" s="75"/>
-      <c r="D167" s="75"/>
-      <c r="E167" s="75"/>
-      <c r="F167" s="75"/>
-      <c r="G167" s="76"/>
+      <c r="C167" s="78"/>
+      <c r="D167" s="78"/>
+      <c r="E167" s="78"/>
+      <c r="F167" s="78"/>
+      <c r="G167" s="79"/>
     </row>
     <row r="168" spans="1:7">
       <c r="A168" s="44" t="s">
@@ -7874,23 +7970,23 @@
       <c r="A174" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="B174" s="77"/>
-      <c r="C174" s="78"/>
-      <c r="D174" s="78"/>
-      <c r="E174" s="78"/>
-      <c r="F174" s="78"/>
-      <c r="G174" s="79"/>
+      <c r="B174" s="71"/>
+      <c r="C174" s="72"/>
+      <c r="D174" s="72"/>
+      <c r="E174" s="72"/>
+      <c r="F174" s="72"/>
+      <c r="G174" s="73"/>
     </row>
     <row r="175" spans="1:7">
       <c r="A175" s="40" t="s">
         <v>187</v>
       </c>
-      <c r="B175" s="71" t="s">
+      <c r="B175" s="74" t="s">
         <v>169</v>
       </c>
-      <c r="C175" s="72"/>
-      <c r="D175" s="72"/>
-      <c r="E175" s="73"/>
+      <c r="C175" s="75"/>
+      <c r="D175" s="75"/>
+      <c r="E175" s="76"/>
       <c r="F175" s="41" t="s">
         <v>54</v>
       </c>
@@ -7903,14 +7999,14 @@
       <c r="A176" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="B176" s="74" t="s">
+      <c r="B176" s="77" t="s">
         <v>71</v>
       </c>
-      <c r="C176" s="75"/>
-      <c r="D176" s="75"/>
-      <c r="E176" s="75"/>
-      <c r="F176" s="75"/>
-      <c r="G176" s="76"/>
+      <c r="C176" s="78"/>
+      <c r="D176" s="78"/>
+      <c r="E176" s="78"/>
+      <c r="F176" s="78"/>
+      <c r="G176" s="79"/>
     </row>
     <row r="177" spans="1:7">
       <c r="A177" s="44" t="s">
@@ -8024,23 +8120,23 @@
       <c r="A183" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="B183" s="77"/>
-      <c r="C183" s="78"/>
-      <c r="D183" s="78"/>
-      <c r="E183" s="78"/>
-      <c r="F183" s="78"/>
-      <c r="G183" s="79"/>
+      <c r="B183" s="71"/>
+      <c r="C183" s="72"/>
+      <c r="D183" s="72"/>
+      <c r="E183" s="72"/>
+      <c r="F183" s="72"/>
+      <c r="G183" s="73"/>
     </row>
     <row r="184" spans="1:7">
       <c r="A184" s="40" t="s">
-        <v>198</v>
-      </c>
-      <c r="B184" s="71" t="s">
+        <v>196</v>
+      </c>
+      <c r="B184" s="74" t="s">
         <v>159</v>
       </c>
-      <c r="C184" s="72"/>
-      <c r="D184" s="72"/>
-      <c r="E184" s="73"/>
+      <c r="C184" s="75"/>
+      <c r="D184" s="75"/>
+      <c r="E184" s="76"/>
       <c r="F184" s="41" t="s">
         <v>54</v>
       </c>
@@ -8053,14 +8149,14 @@
       <c r="A185" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="B185" s="74" t="s">
+      <c r="B185" s="77" t="s">
         <v>71</v>
       </c>
-      <c r="C185" s="75"/>
-      <c r="D185" s="75"/>
-      <c r="E185" s="75"/>
-      <c r="F185" s="75"/>
-      <c r="G185" s="76"/>
+      <c r="C185" s="78"/>
+      <c r="D185" s="78"/>
+      <c r="E185" s="78"/>
+      <c r="F185" s="78"/>
+      <c r="G185" s="79"/>
     </row>
     <row r="186" spans="1:7">
       <c r="A186" s="44" t="s">
@@ -8112,7 +8208,7 @@
         <v>192</v>
       </c>
       <c r="C188" s="47" t="s">
-        <v>193</v>
+        <v>226</v>
       </c>
       <c r="D188" s="47"/>
       <c r="E188" s="47"/>
@@ -8126,10 +8222,10 @@
         <v>3</v>
       </c>
       <c r="B189" s="46" t="s">
-        <v>194</v>
+        <v>225</v>
       </c>
       <c r="C189" s="47" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D189" s="47"/>
       <c r="E189" s="47"/>
@@ -8143,10 +8239,10 @@
         <v>4</v>
       </c>
       <c r="B190" s="46" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C190" s="47" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D190" s="47"/>
       <c r="E190" s="47"/>
@@ -8159,23 +8255,23 @@
       <c r="A191" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="B191" s="77"/>
-      <c r="C191" s="78"/>
-      <c r="D191" s="78"/>
-      <c r="E191" s="78"/>
-      <c r="F191" s="78"/>
-      <c r="G191" s="79"/>
+      <c r="B191" s="71"/>
+      <c r="C191" s="72"/>
+      <c r="D191" s="72"/>
+      <c r="E191" s="72"/>
+      <c r="F191" s="72"/>
+      <c r="G191" s="73"/>
     </row>
     <row r="192" spans="1:7">
       <c r="A192" s="40" t="s">
-        <v>210</v>
-      </c>
-      <c r="B192" s="71" t="s">
-        <v>199</v>
-      </c>
-      <c r="C192" s="72"/>
-      <c r="D192" s="72"/>
-      <c r="E192" s="73"/>
+        <v>208</v>
+      </c>
+      <c r="B192" s="74" t="s">
+        <v>197</v>
+      </c>
+      <c r="C192" s="75"/>
+      <c r="D192" s="75"/>
+      <c r="E192" s="76"/>
       <c r="F192" s="41" t="s">
         <v>54</v>
       </c>
@@ -8188,14 +8284,14 @@
       <c r="A193" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="B193" s="74" t="s">
+      <c r="B193" s="77" t="s">
         <v>71</v>
       </c>
-      <c r="C193" s="75"/>
-      <c r="D193" s="75"/>
-      <c r="E193" s="75"/>
-      <c r="F193" s="75"/>
-      <c r="G193" s="76"/>
+      <c r="C193" s="78"/>
+      <c r="D193" s="78"/>
+      <c r="E193" s="78"/>
+      <c r="F193" s="78"/>
+      <c r="G193" s="79"/>
     </row>
     <row r="194" spans="1:7">
       <c r="A194" s="44" t="s">
@@ -8228,7 +8324,7 @@
         <v>65</v>
       </c>
       <c r="C195" s="47" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D195" s="47"/>
       <c r="E195" s="47"/>
@@ -8242,10 +8338,10 @@
         <v>2</v>
       </c>
       <c r="B196" s="46" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C196" s="47" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D196" s="47"/>
       <c r="E196" s="47"/>
@@ -8259,10 +8355,10 @@
         <v>3</v>
       </c>
       <c r="B197" s="46" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C197" s="47" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D197" s="47"/>
       <c r="E197" s="47"/>
@@ -8276,10 +8372,10 @@
         <v>4</v>
       </c>
       <c r="B198" s="46" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C198" s="47" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D198" s="47"/>
       <c r="E198" s="47"/>
@@ -8293,10 +8389,10 @@
         <v>5</v>
       </c>
       <c r="B199" s="46" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C199" s="47" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D199" s="47"/>
       <c r="E199" s="47"/>
@@ -8309,156 +8405,284 @@
       <c r="A200" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="B200" s="77"/>
-      <c r="C200" s="78"/>
-      <c r="D200" s="78"/>
-      <c r="E200" s="78"/>
-      <c r="F200" s="78"/>
-      <c r="G200" s="79"/>
+      <c r="B200" s="71"/>
+      <c r="C200" s="72"/>
+      <c r="D200" s="72"/>
+      <c r="E200" s="72"/>
+      <c r="F200" s="72"/>
+      <c r="G200" s="73"/>
     </row>
     <row r="201" spans="1:7">
-      <c r="A201" s="16"/>
-      <c r="B201" s="16"/>
-      <c r="C201" s="16"/>
-      <c r="D201" s="16"/>
-      <c r="E201" s="16"/>
-      <c r="F201" s="16"/>
-      <c r="G201" s="16"/>
-    </row>
-    <row r="202" spans="1:7">
-      <c r="A202" s="16"/>
-      <c r="B202" s="16"/>
-      <c r="C202" s="16"/>
-      <c r="D202" s="16"/>
-      <c r="E202" s="16"/>
-      <c r="F202" s="16"/>
-      <c r="G202" s="16"/>
+      <c r="A201" s="40" t="s">
+        <v>214</v>
+      </c>
+      <c r="B201" s="74" t="s">
+        <v>209</v>
+      </c>
+      <c r="C201" s="75"/>
+      <c r="D201" s="75"/>
+      <c r="E201" s="76"/>
+      <c r="F201" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="G201" s="42" t="str">
+        <f>IF(COUNTIF(F204:F208,"Blocked")&gt;0,"Blocked",IF(COUNTIF(F204:F208,"Fail")&gt;0,"Fail",IF(COUNTIF(F204:F208,"")=0,"Pass","Not Executed")))</f>
+        <v>Fail</v>
+      </c>
+    </row>
+    <row r="202" spans="1:7" ht="15" customHeight="1">
+      <c r="A202" s="43" t="s">
+        <v>56</v>
+      </c>
+      <c r="B202" s="77" t="s">
+        <v>71</v>
+      </c>
+      <c r="C202" s="78"/>
+      <c r="D202" s="78"/>
+      <c r="E202" s="78"/>
+      <c r="F202" s="78"/>
+      <c r="G202" s="79"/>
     </row>
     <row r="203" spans="1:7">
-      <c r="A203" s="16"/>
-      <c r="B203" s="16"/>
-      <c r="C203" s="16"/>
-      <c r="D203" s="16"/>
-      <c r="E203" s="16"/>
-      <c r="F203" s="16"/>
-      <c r="G203" s="16"/>
-    </row>
-    <row r="204" spans="1:7">
-      <c r="A204" s="16"/>
-      <c r="B204" s="16"/>
-      <c r="C204" s="16"/>
-      <c r="D204" s="16"/>
-      <c r="E204" s="16"/>
-      <c r="F204" s="16"/>
-      <c r="G204" s="16"/>
-    </row>
-    <row r="205" spans="1:7">
-      <c r="A205" s="16"/>
-      <c r="B205" s="16"/>
-      <c r="C205" s="16"/>
-      <c r="D205" s="16"/>
-      <c r="E205" s="16"/>
-      <c r="F205" s="16"/>
-      <c r="G205" s="16"/>
-    </row>
-    <row r="206" spans="1:7">
-      <c r="A206" s="16"/>
-      <c r="B206" s="16"/>
-      <c r="C206" s="16"/>
-      <c r="D206" s="16"/>
-      <c r="E206" s="16"/>
-      <c r="F206" s="16"/>
-      <c r="G206" s="16"/>
-    </row>
-    <row r="207" spans="1:7">
-      <c r="A207" s="16"/>
-      <c r="B207" s="16"/>
-      <c r="C207" s="16"/>
-      <c r="D207" s="16"/>
-      <c r="E207" s="16"/>
-      <c r="F207" s="16"/>
-      <c r="G207" s="16"/>
-    </row>
-    <row r="208" spans="1:7">
-      <c r="A208" s="16"/>
-      <c r="B208" s="16"/>
-      <c r="C208" s="16"/>
-      <c r="D208" s="16"/>
-      <c r="E208" s="16"/>
-      <c r="F208" s="16"/>
-      <c r="G208" s="16"/>
+      <c r="A203" s="44" t="s">
+        <v>58</v>
+      </c>
+      <c r="B203" s="44" t="s">
+        <v>59</v>
+      </c>
+      <c r="C203" s="44" t="s">
+        <v>60</v>
+      </c>
+      <c r="D203" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="E203" s="44" t="s">
+        <v>62</v>
+      </c>
+      <c r="F203" s="44" t="s">
+        <v>63</v>
+      </c>
+      <c r="G203" s="44" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="204" spans="1:7" ht="165">
+      <c r="A204" s="45">
+        <v>1</v>
+      </c>
+      <c r="B204" s="46" t="s">
+        <v>65</v>
+      </c>
+      <c r="C204" s="47" t="s">
+        <v>199</v>
+      </c>
+      <c r="D204" s="47" t="s">
+        <v>216</v>
+      </c>
+      <c r="E204" s="47"/>
+      <c r="F204" s="48" t="s">
+        <v>4</v>
+      </c>
+      <c r="G204" s="49"/>
+    </row>
+    <row r="205" spans="1:7" ht="15.75">
+      <c r="A205" s="45">
+        <v>2</v>
+      </c>
+      <c r="B205" s="46" t="s">
+        <v>217</v>
+      </c>
+      <c r="C205" s="47" t="s">
+        <v>218</v>
+      </c>
+      <c r="D205" s="47"/>
+      <c r="E205" s="47"/>
+      <c r="F205" s="48" t="s">
+        <v>4</v>
+      </c>
+      <c r="G205" s="49"/>
+    </row>
+    <row r="206" spans="1:7" ht="15.75">
+      <c r="A206" s="45">
+        <v>3</v>
+      </c>
+      <c r="B206" s="46" t="s">
+        <v>219</v>
+      </c>
+      <c r="C206" s="47" t="s">
+        <v>220</v>
+      </c>
+      <c r="D206" s="47"/>
+      <c r="E206" s="47"/>
+      <c r="F206" s="48" t="s">
+        <v>4</v>
+      </c>
+      <c r="G206" s="49"/>
+    </row>
+    <row r="207" spans="1:7" ht="15.75">
+      <c r="A207" s="45">
+        <v>4</v>
+      </c>
+      <c r="B207" s="46" t="s">
+        <v>221</v>
+      </c>
+      <c r="C207" s="47" t="s">
+        <v>222</v>
+      </c>
+      <c r="D207" s="47"/>
+      <c r="E207" s="47"/>
+      <c r="F207" s="48" t="s">
+        <v>4</v>
+      </c>
+      <c r="G207" s="49"/>
+    </row>
+    <row r="208" spans="1:7" ht="45">
+      <c r="A208" s="45">
+        <v>5</v>
+      </c>
+      <c r="B208" s="46" t="s">
+        <v>223</v>
+      </c>
+      <c r="C208" s="47" t="s">
+        <v>224</v>
+      </c>
+      <c r="D208" s="47"/>
+      <c r="E208" s="47"/>
+      <c r="F208" s="48" t="s">
+        <v>5</v>
+      </c>
+      <c r="G208" s="49"/>
     </row>
     <row r="209" spans="1:7">
-      <c r="A209" s="16"/>
-      <c r="B209" s="16"/>
-      <c r="C209" s="16"/>
-      <c r="D209" s="16"/>
-      <c r="E209" s="16"/>
-      <c r="F209" s="16"/>
-      <c r="G209" s="16"/>
+      <c r="A209" s="50" t="s">
+        <v>66</v>
+      </c>
+      <c r="B209" s="71"/>
+      <c r="C209" s="72"/>
+      <c r="D209" s="72"/>
+      <c r="E209" s="72"/>
+      <c r="F209" s="72"/>
+      <c r="G209" s="73"/>
     </row>
     <row r="210" spans="1:7">
-      <c r="A210" s="16"/>
-      <c r="B210" s="16"/>
-      <c r="C210" s="16"/>
-      <c r="D210" s="16"/>
-      <c r="E210" s="16"/>
-      <c r="F210" s="16"/>
-      <c r="G210" s="16"/>
-    </row>
-    <row r="211" spans="1:7">
-      <c r="A211" s="16"/>
-      <c r="B211" s="16"/>
-      <c r="C211" s="16"/>
-      <c r="D211" s="16"/>
-      <c r="E211" s="16"/>
-      <c r="F211" s="16"/>
-      <c r="G211" s="16"/>
+      <c r="A210" s="40" t="s">
+        <v>227</v>
+      </c>
+      <c r="B210" s="74" t="s">
+        <v>212</v>
+      </c>
+      <c r="C210" s="75"/>
+      <c r="D210" s="75"/>
+      <c r="E210" s="76"/>
+      <c r="F210" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="G210" s="42" t="str">
+        <f>IF(COUNTIF(F213:F215,"Blocked")&gt;0,"Blocked",IF(COUNTIF(F213:F215,"Fail")&gt;0,"Fail",IF(COUNTIF(F213:F215,"")=0,"Pass","Not Executed")))</f>
+        <v>Fail</v>
+      </c>
+    </row>
+    <row r="211" spans="1:7" ht="15" customHeight="1">
+      <c r="A211" s="43" t="s">
+        <v>56</v>
+      </c>
+      <c r="B211" s="77" t="s">
+        <v>71</v>
+      </c>
+      <c r="C211" s="78"/>
+      <c r="D211" s="78"/>
+      <c r="E211" s="78"/>
+      <c r="F211" s="78"/>
+      <c r="G211" s="79"/>
     </row>
     <row r="212" spans="1:7">
-      <c r="A212" s="16"/>
-      <c r="B212" s="16"/>
-      <c r="C212" s="16"/>
-      <c r="D212" s="16"/>
-      <c r="E212" s="16"/>
-      <c r="F212" s="16"/>
-      <c r="G212" s="16"/>
-    </row>
-    <row r="213" spans="1:7">
-      <c r="A213" s="16"/>
-      <c r="B213" s="16"/>
-      <c r="C213" s="16"/>
-      <c r="D213" s="16"/>
-      <c r="E213" s="16"/>
-      <c r="F213" s="16"/>
-      <c r="G213" s="16"/>
-    </row>
-    <row r="214" spans="1:7">
-      <c r="A214" s="16"/>
-      <c r="B214" s="16"/>
-      <c r="C214" s="16"/>
-      <c r="D214" s="16"/>
-      <c r="E214" s="16"/>
-      <c r="F214" s="16"/>
-      <c r="G214" s="16"/>
-    </row>
-    <row r="215" spans="1:7">
-      <c r="A215" s="16"/>
-      <c r="B215" s="16"/>
-      <c r="C215" s="16"/>
-      <c r="D215" s="16"/>
-      <c r="E215" s="16"/>
-      <c r="F215" s="16"/>
-      <c r="G215" s="16"/>
+      <c r="A212" s="44" t="s">
+        <v>58</v>
+      </c>
+      <c r="B212" s="44" t="s">
+        <v>59</v>
+      </c>
+      <c r="C212" s="44" t="s">
+        <v>60</v>
+      </c>
+      <c r="D212" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="E212" s="44" t="s">
+        <v>62</v>
+      </c>
+      <c r="F212" s="44" t="s">
+        <v>63</v>
+      </c>
+      <c r="G212" s="44" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="213" spans="1:7" ht="165">
+      <c r="A213" s="45">
+        <v>1</v>
+      </c>
+      <c r="B213" s="46" t="s">
+        <v>65</v>
+      </c>
+      <c r="C213" s="47" t="s">
+        <v>199</v>
+      </c>
+      <c r="D213" s="47" t="s">
+        <v>216</v>
+      </c>
+      <c r="E213" s="47"/>
+      <c r="F213" s="48" t="s">
+        <v>4</v>
+      </c>
+      <c r="G213" s="49"/>
+    </row>
+    <row r="214" spans="1:7" ht="45">
+      <c r="A214" s="45">
+        <v>2</v>
+      </c>
+      <c r="B214" s="46" t="s">
+        <v>228</v>
+      </c>
+      <c r="C214" s="47" t="s">
+        <v>229</v>
+      </c>
+      <c r="D214" s="47"/>
+      <c r="E214" s="47"/>
+      <c r="F214" s="48" t="s">
+        <v>4</v>
+      </c>
+      <c r="G214" s="49"/>
+    </row>
+    <row r="215" spans="1:7" ht="45">
+      <c r="A215" s="45">
+        <v>3</v>
+      </c>
+      <c r="B215" s="46" t="s">
+        <v>230</v>
+      </c>
+      <c r="C215" s="47" t="s">
+        <v>229</v>
+      </c>
+      <c r="D215" s="47"/>
+      <c r="E215" s="47"/>
+      <c r="F215" s="48" t="s">
+        <v>5</v>
+      </c>
+      <c r="G215" s="46" t="s">
+        <v>231</v>
+      </c>
     </row>
     <row r="216" spans="1:7">
-      <c r="A216" s="16"/>
-      <c r="B216" s="16"/>
-      <c r="C216" s="16"/>
-      <c r="D216" s="16"/>
-      <c r="E216" s="16"/>
-      <c r="F216" s="16"/>
-      <c r="G216" s="16"/>
+      <c r="A216" s="50" t="s">
+        <v>66</v>
+      </c>
+      <c r="B216" s="71"/>
+      <c r="C216" s="72"/>
+      <c r="D216" s="72"/>
+      <c r="E216" s="72"/>
+      <c r="F216" s="72"/>
+      <c r="G216" s="73"/>
     </row>
     <row r="217" spans="1:7">
       <c r="A217" s="16"/>
@@ -9810,39 +10034,39 @@
       <c r="F366" s="16"/>
       <c r="G366" s="16"/>
     </row>
-    <row r="367" spans="1:7">
-      <c r="A367" s="16"/>
-      <c r="B367" s="16"/>
-      <c r="C367" s="16"/>
-      <c r="D367" s="16"/>
-      <c r="E367" s="16"/>
-      <c r="F367" s="16"/>
-      <c r="G367" s="16"/>
-    </row>
-    <row r="368" spans="1:7">
-      <c r="A368" s="16"/>
-      <c r="B368" s="16"/>
-      <c r="C368" s="16"/>
-      <c r="D368" s="16"/>
-      <c r="E368" s="16"/>
-      <c r="F368" s="16"/>
-      <c r="G368" s="16"/>
-    </row>
-    <row r="369" spans="1:8" ht="15.75">
+    <row r="367" spans="1:7" ht="15.75">
+      <c r="A367" s="13"/>
+      <c r="B367" s="33"/>
+      <c r="C367" s="33"/>
+      <c r="D367" s="53"/>
+      <c r="E367" s="54"/>
+      <c r="F367" s="55"/>
+    </row>
+    <row r="368" spans="1:7" ht="15.75">
+      <c r="A368" s="13"/>
+      <c r="B368" s="33"/>
+      <c r="C368" s="33"/>
+      <c r="D368" s="53"/>
+      <c r="E368" s="54"/>
+      <c r="F368" s="55"/>
+    </row>
+    <row r="369" spans="1:8" s="34" customFormat="1" ht="15.75">
       <c r="A369" s="13"/>
       <c r="B369" s="33"/>
       <c r="C369" s="33"/>
       <c r="D369" s="53"/>
       <c r="E369" s="54"/>
       <c r="F369" s="55"/>
-    </row>
-    <row r="370" spans="1:8" ht="15.75">
+      <c r="H369" s="12"/>
+    </row>
+    <row r="370" spans="1:8" s="34" customFormat="1" ht="15.75">
       <c r="A370" s="13"/>
       <c r="B370" s="33"/>
       <c r="C370" s="33"/>
       <c r="D370" s="53"/>
       <c r="E370" s="54"/>
       <c r="F370" s="55"/>
+      <c r="H370" s="12"/>
     </row>
     <row r="371" spans="1:8" s="34" customFormat="1" ht="15.75">
       <c r="A371" s="13"/>
@@ -14470,45 +14694,62 @@
       <c r="F884" s="55"/>
       <c r="H884" s="12"/>
     </row>
-    <row r="885" spans="1:8" s="34" customFormat="1" ht="15.75">
-      <c r="A885" s="13"/>
-      <c r="B885" s="33"/>
-      <c r="C885" s="33"/>
-      <c r="D885" s="53"/>
-      <c r="E885" s="54"/>
-      <c r="F885" s="55"/>
-      <c r="H885" s="12"/>
-    </row>
-    <row r="886" spans="1:8" s="34" customFormat="1" ht="15.75">
-      <c r="A886" s="13"/>
-      <c r="B886" s="33"/>
-      <c r="C886" s="33"/>
-      <c r="D886" s="53"/>
-      <c r="E886" s="54"/>
-      <c r="F886" s="55"/>
-      <c r="H886" s="12"/>
-    </row>
   </sheetData>
-  <mergeCells count="76">
-    <mergeCell ref="B132:G132"/>
-    <mergeCell ref="B118:E118"/>
-    <mergeCell ref="B119:G119"/>
-    <mergeCell ref="B124:G124"/>
-    <mergeCell ref="B125:E125"/>
-    <mergeCell ref="B126:G126"/>
-    <mergeCell ref="B112:E112"/>
-    <mergeCell ref="B113:G113"/>
-    <mergeCell ref="B117:G117"/>
-    <mergeCell ref="B104:E104"/>
-    <mergeCell ref="B105:G105"/>
-    <mergeCell ref="B111:G111"/>
-    <mergeCell ref="B96:E96"/>
-    <mergeCell ref="B97:G97"/>
-    <mergeCell ref="B103:G103"/>
-    <mergeCell ref="B87:G87"/>
-    <mergeCell ref="B88:E88"/>
-    <mergeCell ref="B89:G89"/>
-    <mergeCell ref="B95:G95"/>
+  <mergeCells count="82">
+    <mergeCell ref="B216:G216"/>
+    <mergeCell ref="B201:E201"/>
+    <mergeCell ref="B202:G202"/>
+    <mergeCell ref="B209:G209"/>
+    <mergeCell ref="B210:E210"/>
+    <mergeCell ref="B211:G211"/>
+    <mergeCell ref="B192:E192"/>
+    <mergeCell ref="B193:G193"/>
+    <mergeCell ref="B200:G200"/>
+    <mergeCell ref="B191:G191"/>
+    <mergeCell ref="B175:E175"/>
+    <mergeCell ref="B176:G176"/>
+    <mergeCell ref="B183:G183"/>
+    <mergeCell ref="B184:E184"/>
+    <mergeCell ref="B185:G185"/>
+    <mergeCell ref="B158:G158"/>
+    <mergeCell ref="B165:G165"/>
+    <mergeCell ref="B166:E166"/>
+    <mergeCell ref="B167:G167"/>
+    <mergeCell ref="B174:G174"/>
+    <mergeCell ref="B148:G148"/>
+    <mergeCell ref="B149:E149"/>
+    <mergeCell ref="B150:G150"/>
+    <mergeCell ref="B156:G156"/>
+    <mergeCell ref="B157:E157"/>
+    <mergeCell ref="B133:E133"/>
+    <mergeCell ref="B134:G134"/>
+    <mergeCell ref="B140:G140"/>
+    <mergeCell ref="B141:E141"/>
+    <mergeCell ref="B142:G142"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="A16:G16"/>
+    <mergeCell ref="A17:G17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B38:G38"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="B31:G31"/>
+    <mergeCell ref="B36:G36"/>
+    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="B58:G58"/>
+    <mergeCell ref="B43:G43"/>
+    <mergeCell ref="B44:E44"/>
+    <mergeCell ref="B45:G45"/>
+    <mergeCell ref="B49:G49"/>
+    <mergeCell ref="B50:E50"/>
+    <mergeCell ref="B51:G51"/>
+    <mergeCell ref="B56:G56"/>
+    <mergeCell ref="B57:E57"/>
     <mergeCell ref="B81:G81"/>
     <mergeCell ref="B63:G63"/>
     <mergeCell ref="B72:E72"/>
@@ -14518,57 +14759,28 @@
     <mergeCell ref="B64:E64"/>
     <mergeCell ref="B65:G65"/>
     <mergeCell ref="B71:G71"/>
-    <mergeCell ref="B58:G58"/>
-    <mergeCell ref="B43:G43"/>
-    <mergeCell ref="B44:E44"/>
-    <mergeCell ref="B45:G45"/>
-    <mergeCell ref="B49:G49"/>
-    <mergeCell ref="B50:E50"/>
-    <mergeCell ref="B51:G51"/>
-    <mergeCell ref="B56:G56"/>
-    <mergeCell ref="B57:E57"/>
-    <mergeCell ref="B38:G38"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="B31:G31"/>
-    <mergeCell ref="B36:G36"/>
-    <mergeCell ref="B37:E37"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="A16:G16"/>
-    <mergeCell ref="A17:G17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B133:E133"/>
-    <mergeCell ref="B134:G134"/>
-    <mergeCell ref="B140:G140"/>
-    <mergeCell ref="B141:E141"/>
-    <mergeCell ref="B142:G142"/>
-    <mergeCell ref="B148:G148"/>
-    <mergeCell ref="B149:E149"/>
-    <mergeCell ref="B150:G150"/>
-    <mergeCell ref="B156:G156"/>
-    <mergeCell ref="B157:E157"/>
-    <mergeCell ref="B158:G158"/>
-    <mergeCell ref="B165:G165"/>
-    <mergeCell ref="B166:E166"/>
-    <mergeCell ref="B167:G167"/>
-    <mergeCell ref="B174:G174"/>
-    <mergeCell ref="B192:E192"/>
-    <mergeCell ref="B193:G193"/>
-    <mergeCell ref="B200:G200"/>
-    <mergeCell ref="B191:G191"/>
-    <mergeCell ref="B175:E175"/>
-    <mergeCell ref="B176:G176"/>
-    <mergeCell ref="B183:G183"/>
-    <mergeCell ref="B184:E184"/>
-    <mergeCell ref="B185:G185"/>
+    <mergeCell ref="B96:E96"/>
+    <mergeCell ref="B97:G97"/>
+    <mergeCell ref="B103:G103"/>
+    <mergeCell ref="B87:G87"/>
+    <mergeCell ref="B88:E88"/>
+    <mergeCell ref="B89:G89"/>
+    <mergeCell ref="B95:G95"/>
+    <mergeCell ref="B112:E112"/>
+    <mergeCell ref="B113:G113"/>
+    <mergeCell ref="B117:G117"/>
+    <mergeCell ref="B104:E104"/>
+    <mergeCell ref="B105:G105"/>
+    <mergeCell ref="B111:G111"/>
+    <mergeCell ref="B132:G132"/>
+    <mergeCell ref="B118:E118"/>
+    <mergeCell ref="B119:G119"/>
+    <mergeCell ref="B124:G124"/>
+    <mergeCell ref="B125:E125"/>
+    <mergeCell ref="B126:G126"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" showErrorMessage="1" promptTitle="Valid values include:" prompt="_x000a_" sqref="F369:F371 F376:F382 F595:F597 F585:F590 F387:F396 F401:F404 F409:F414 F419:F427 F432:F441 F446:F456 F461:F471 F487:F493 F515:F517 F476:F482 F498:F504 F509:F510 F522:F528 F533:F539 F555:F557 F544:F550 F562:F565 F570:F572 F577:F580 F21 F107:F110 F67:F70 F75:F78 F26:F28 F40:F42 F33:F35 F47:F49 F53:F55 F60:F62 F83:F86 F91:F94 F99:F102 F115:F116 F121:F123 F128:F131 F136:F139 F144:F147 F152:F155 F160:F164 F169:F173 F178:F182 F187:F190 F195:F199">
+    <dataValidation type="list" showErrorMessage="1" promptTitle="Valid values include:" prompt="_x000a_" sqref="F367:F369 F374:F380 F593:F595 F583:F588 F385:F394 F399:F402 F407:F412 F417:F425 F430:F439 F444:F454 F459:F469 F485:F491 F513:F515 F474:F480 F496:F502 F507:F508 F520:F526 F531:F537 F553:F555 F542:F548 F560:F563 F568:F570 F575:F578 F213:F215 F204:F208 F195:F199 F187:F190 F178:F182 F169:F173 F160:F164 F152:F155 F144:F147 F136:F139 F128:F131 F121:F123 F115:F116 F99:F102 F91:F94 F83:F86 F60:F62 F53:F55 F47:F49 F33:F35 F40:F42 F26:F28 F75:F78 F67:F70 F107:F110 F21">
       <formula1>"Pass, Fail, Blocked"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Pivot Remarks : cases added 48 Summary Tag : Cases added 25,26 New fun - SSO login
</commit_message>
<xml_diff>
--- a/TCS_NEWUI-Export.xlsx
+++ b/TCS_NEWUI-Export.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4506"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sumit Rana\Projects\AdIntel- New\Test Cases\TC Repository\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3687E5AC-6155-431C-8767-83A217C51F24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="12240" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="2" r:id="rId1"/>
@@ -35,9 +41,9 @@
     <definedName name="test" localSheetId="2">#REF!</definedName>
     <definedName name="test">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -820,7 +826,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
@@ -1760,23 +1766,23 @@
     </xf>
   </cellXfs>
   <cellStyles count="17">
-    <cellStyle name="40% - Accent2 2 3 2 2" xfId="9"/>
-    <cellStyle name="Accent1 2 2 2 2 3" xfId="7"/>
-    <cellStyle name="Accent1 2 3 2 2" xfId="3"/>
-    <cellStyle name="Accent2 2 3 2 2" xfId="4"/>
-    <cellStyle name="Comma [0] 2" xfId="15"/>
-    <cellStyle name="Comma [0] 3" xfId="16"/>
-    <cellStyle name="Heading 2 2 2 2 2 3 2" xfId="8"/>
+    <cellStyle name="40% - Accent2 2 3 2 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Accent1 2 2 2 2 3" xfId="7" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Accent1 2 3 2 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Accent2 2 3 2 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Comma [0] 2" xfId="15" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Comma [0] 3" xfId="16" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Heading 2 2 2 2 2 3 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Hyperlink 2" xfId="5"/>
+    <cellStyle name="Hyperlink 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="13"/>
-    <cellStyle name="Normal 2 4 2" xfId="2"/>
-    <cellStyle name="Normal 3 2 4 2" xfId="6"/>
-    <cellStyle name="Normal 3 2 4 3 2" xfId="11"/>
-    <cellStyle name="Normal 6" xfId="10"/>
-    <cellStyle name="TableStyleLight1 3 4 2" xfId="14"/>
-    <cellStyle name="TableStyleLight1 3 4 3 2" xfId="12"/>
+    <cellStyle name="Normal 2" xfId="13" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Normal 2 4 2" xfId="2" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="Normal 3 2 4 2" xfId="6" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="Normal 3 2 4 3 2" xfId="11" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="Normal 6" xfId="10" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="TableStyleLight1 3 4 2" xfId="14" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="TableStyleLight1 3 4 3 2" xfId="12" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1792,10 +1798,18 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="1"/>
-  <c:style val="48"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="148"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="48"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1818,7 +1832,9 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -1834,6 +1850,7 @@
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1848,8 +1865,11 @@
               <a:bevelT w="63500" h="25400"/>
             </a:sp3d>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:dPt>
             <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent3">
@@ -1866,7 +1886,7 @@
                 <a:bevelT w="63500" h="25400"/>
               </a:sp3d>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-8970-41E1-9689-13CA975A75E2}"/>
               </c:ext>
@@ -1874,6 +1894,8 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="E22B00"/>
@@ -1888,7 +1910,7 @@
                 <a:bevelT w="63500" h="25400"/>
               </a:sp3d>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-8970-41E1-9689-13CA975A75E2}"/>
               </c:ext>
@@ -1896,6 +1918,8 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="FFC000"/>
@@ -1910,7 +1934,7 @@
                 <a:bevelT w="63500" h="25400"/>
               </a:sp3d>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000005-8970-41E1-9689-13CA975A75E2}"/>
               </c:ext>
@@ -1918,6 +1942,8 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="00B0F0"/>
@@ -1932,7 +1958,7 @@
                 <a:bevelT w="63500" h="25400"/>
               </a:sp3d>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000007-8970-41E1-9689-13CA975A75E2}"/>
               </c:ext>
@@ -1956,8 +1982,14 @@
                 <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
+            <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -2004,12 +2036,21 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000008-8970-41E1-9689-13CA975A75E2}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
         <c:axId val="52209152"/>
         <c:axId val="52210688"/>
       </c:barChart>
@@ -2018,8 +2059,11 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
@@ -2038,6 +2082,7 @@
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="52210688"/>
@@ -2047,6 +2092,8 @@
         <c:delete val="1"/>
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
         <c:crossAx val="52209152"/>
         <c:crosses val="autoZero"/>
@@ -2055,6 +2102,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:effectLst/>
@@ -2075,10 +2123,18 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="1"/>
-  <c:style val="45"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="145"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="45"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -2101,12 +2157,24 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:view3D>
       <c:rotX val="30"/>
       <c:rotY val="32"/>
+      <c:rAngAx val="0"/>
       <c:perspective val="90"/>
     </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+    </c:backWall>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -2126,6 +2194,7 @@
           <c:order val="0"/>
           <c:dPt>
             <c:idx val="0"/>
+            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent3">
@@ -2134,7 +2203,7 @@
                 </a:schemeClr>
               </a:solidFill>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-5019-4889-AF25-FEA016BCB8F3}"/>
               </c:ext>
@@ -2142,6 +2211,7 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
+            <c:bubble3D val="0"/>
             <c:explosion val="19"/>
             <c:spPr>
               <a:solidFill>
@@ -2151,7 +2221,7 @@
                 </a:schemeClr>
               </a:solidFill>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-5019-4889-AF25-FEA016BCB8F3}"/>
               </c:ext>
@@ -2175,6 +2245,17 @@
                   <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-5019-4889-AF25-FEA016BCB8F3}"/>
+                </c:ext>
+              </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
@@ -2193,6 +2274,17 @@
                   <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-5019-4889-AF25-FEA016BCB8F3}"/>
+                </c:ext>
+              </c:extLst>
             </c:dLbl>
             <c:spPr>
               <a:noFill/>
@@ -2201,9 +2293,14 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
             <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="1"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
@@ -2236,14 +2333,20 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-5019-4889-AF25-FEA016BCB8F3}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
           <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
         </c:dLbls>
       </c:pie3DChart>
       <c:spPr>
@@ -2264,9 +2367,11 @@
           <c:h val="7.1280252974084315E-2"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:ln w="0"/>
@@ -2288,9 +2393,20 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -2315,6 +2431,7 @@
           </c:spPr>
           <c:dPt>
             <c:idx val="0"/>
+            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="92D050"/>
@@ -2323,7 +2440,7 @@
                 <a:noFill/>
               </a:ln>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-B540-41C7-94E0-A9CBA388CE63}"/>
               </c:ext>
@@ -2331,6 +2448,7 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
+            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
@@ -2339,7 +2457,7 @@
                 <a:noFill/>
               </a:ln>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-B540-41C7-94E0-A9CBA388CE63}"/>
               </c:ext>
@@ -2347,6 +2465,7 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
+            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="FFC000"/>
@@ -2355,7 +2474,7 @@
                 <a:noFill/>
               </a:ln>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000005-B540-41C7-94E0-A9CBA388CE63}"/>
               </c:ext>
@@ -2363,6 +2482,7 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
+            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="00B0F0"/>
@@ -2371,7 +2491,7 @@
                 <a:noFill/>
               </a:ln>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000007-B540-41C7-94E0-A9CBA388CE63}"/>
               </c:ext>
@@ -2418,12 +2538,21 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000008-B540-41C7-94E0-A9CBA388CE63}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
         <c:firstSliceAng val="0"/>
       </c:pieChart>
       <c:spPr>
@@ -2510,6 +2639,7 @@
           <c:h val="0.95693837006674254"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln w="25400">
@@ -2536,6 +2666,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2593,7 +2724,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2BE14715-47DA-4F23-BAF5-24D2A024087A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2BE14715-47DA-4F23-BAF5-24D2A024087A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2631,7 +2762,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E23D74E-C8F9-4086-8A84-7BF83C5152BB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E23D74E-C8F9-4086-8A84-7BF83C5152BB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2669,7 +2800,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9ABF8EF7-8DD9-44DF-9280-7163A445B39C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9ABF8EF7-8DD9-44DF-9280-7163A445B39C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2681,7 +2812,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -2701,7 +2832,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2772,7 +2903,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60D52198-D506-4AA7-A57B-A8C3D0247DFE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60D52198-D506-4AA7-A57B-A8C3D0247DFE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2784,7 +2915,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -2828,7 +2959,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53DA16D2-291A-42A6-94EB-D697846FA36C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53DA16D2-291A-42A6-94EB-D697846FA36C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2962,7 +3093,7 @@
         </a:effectLst>
         <a:extLst>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525" cmpd="sng">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525" cmpd="sng">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -3012,7 +3143,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C9D5358-04D5-45A9-9117-839674A38F39}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C9D5358-04D5-45A9-9117-839674A38F39}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3050,7 +3181,7 @@
         <xdr:cNvPr id="11" name="Picture 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5460449-34D4-472A-97B4-74063FD93EF7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5460449-34D4-472A-97B4-74063FD93EF7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3060,7 +3191,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3098,7 +3229,7 @@
         <xdr:cNvPr id="15" name="Picture 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3257AE9-B407-40BD-AFE3-45B7CF3B360C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3257AE9-B407-40BD-AFE3-45B7CF3B360C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3108,7 +3239,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3146,7 +3277,7 @@
         <xdr:cNvPr id="22" name="Picture 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BCA27E28-A006-440E-A37D-4323F3CD8901}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BCA27E28-A006-440E-A37D-4323F3CD8901}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3156,7 +3287,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3194,7 +3325,7 @@
         <xdr:cNvPr id="24" name="Picture 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B788E05D-6796-473C-B2C7-EEF8C7A50B05}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B788E05D-6796-473C-B2C7-EEF8C7A50B05}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3206,7 +3337,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3244,7 +3375,7 @@
         <xdr:cNvPr id="26" name="Picture 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3A26610-B5E8-4FA3-BED3-4A266BF78BCD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3A26610-B5E8-4FA3-BED3-4A266BF78BCD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3256,7 +3387,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3294,7 +3425,7 @@
         <xdr:cNvPr id="28" name="Picture 27">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4521285-625F-4CA6-8FC5-4AFAFDF893A8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4521285-625F-4CA6-8FC5-4AFAFDF893A8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3306,7 +3437,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3344,7 +3475,7 @@
         <xdr:cNvPr id="29" name="Picture 28">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89936818-308B-4951-8C43-6322C73A3E3C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89936818-308B-4951-8C43-6322C73A3E3C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3356,7 +3487,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3394,7 +3525,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B80C1EBE-F954-4FAF-9777-6966156D6D68}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B80C1EBE-F954-4FAF-9777-6966156D6D68}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3406,7 +3537,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3444,7 +3575,7 @@
         <xdr:cNvPr id="27" name="Picture 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA25FA63-0A56-4155-9D0A-415548BF2225}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA25FA63-0A56-4155-9D0A-415548BF2225}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3456,7 +3587,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3489,7 +3620,7 @@
         <xdr:cNvPr id="30" name="Picture 29">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A407F95F-057E-476B-A252-51550475ED54}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A407F95F-057E-476B-A252-51550475ED54}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3501,7 +3632,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3534,7 +3665,7 @@
         <xdr:cNvPr id="31" name="Picture 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1BA4C48-C2DC-4892-9738-3F8B87144095}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1BA4C48-C2DC-4892-9738-3F8B87144095}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3546,7 +3677,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3584,7 +3715,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{482A5AC2-E046-43EF-BB61-1DE7A7A1D4FB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{482A5AC2-E046-43EF-BB61-1DE7A7A1D4FB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3596,7 +3727,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3629,7 +3760,7 @@
         <xdr:cNvPr id="35" name="Picture 34">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63ADD56B-1BEA-4C18-896D-3A7E838FC08B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63ADD56B-1BEA-4C18-896D-3A7E838FC08B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3641,7 +3772,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3953,14 +4084,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A5:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4106,7 +4237,7 @@
     <mergeCell ref="G6:G7"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A8" location="'SMART- Export'!A1" display="SMART-Export"/>
+    <hyperlink ref="A8" location="'SMART- Export'!A1" display="SMART-Export" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4115,11 +4246,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.85546875" defaultRowHeight="15"/>
@@ -4471,7 +4602,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I884"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
@@ -14696,12 +14827,73 @@
     </row>
   </sheetData>
   <mergeCells count="82">
-    <mergeCell ref="B216:G216"/>
-    <mergeCell ref="B201:E201"/>
-    <mergeCell ref="B202:G202"/>
-    <mergeCell ref="B209:G209"/>
-    <mergeCell ref="B210:E210"/>
-    <mergeCell ref="B211:G211"/>
+    <mergeCell ref="B132:G132"/>
+    <mergeCell ref="B118:E118"/>
+    <mergeCell ref="B119:G119"/>
+    <mergeCell ref="B124:G124"/>
+    <mergeCell ref="B125:E125"/>
+    <mergeCell ref="B126:G126"/>
+    <mergeCell ref="B112:E112"/>
+    <mergeCell ref="B113:G113"/>
+    <mergeCell ref="B117:G117"/>
+    <mergeCell ref="B104:E104"/>
+    <mergeCell ref="B105:G105"/>
+    <mergeCell ref="B111:G111"/>
+    <mergeCell ref="B96:E96"/>
+    <mergeCell ref="B97:G97"/>
+    <mergeCell ref="B103:G103"/>
+    <mergeCell ref="B87:G87"/>
+    <mergeCell ref="B88:E88"/>
+    <mergeCell ref="B89:G89"/>
+    <mergeCell ref="B95:G95"/>
+    <mergeCell ref="B81:G81"/>
+    <mergeCell ref="B63:G63"/>
+    <mergeCell ref="B72:E72"/>
+    <mergeCell ref="B73:G73"/>
+    <mergeCell ref="B79:G79"/>
+    <mergeCell ref="B80:E80"/>
+    <mergeCell ref="B64:E64"/>
+    <mergeCell ref="B65:G65"/>
+    <mergeCell ref="B71:G71"/>
+    <mergeCell ref="B58:G58"/>
+    <mergeCell ref="B43:G43"/>
+    <mergeCell ref="B44:E44"/>
+    <mergeCell ref="B45:G45"/>
+    <mergeCell ref="B49:G49"/>
+    <mergeCell ref="B50:E50"/>
+    <mergeCell ref="B51:G51"/>
+    <mergeCell ref="B56:G56"/>
+    <mergeCell ref="B57:E57"/>
+    <mergeCell ref="B38:G38"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="B31:G31"/>
+    <mergeCell ref="B36:G36"/>
+    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="A16:G16"/>
+    <mergeCell ref="A17:G17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B133:E133"/>
+    <mergeCell ref="B134:G134"/>
+    <mergeCell ref="B140:G140"/>
+    <mergeCell ref="B141:E141"/>
+    <mergeCell ref="B142:G142"/>
+    <mergeCell ref="B148:G148"/>
+    <mergeCell ref="B149:E149"/>
+    <mergeCell ref="B150:G150"/>
+    <mergeCell ref="B156:G156"/>
+    <mergeCell ref="B157:E157"/>
+    <mergeCell ref="B158:G158"/>
+    <mergeCell ref="B165:G165"/>
+    <mergeCell ref="B166:E166"/>
+    <mergeCell ref="B167:G167"/>
+    <mergeCell ref="B174:G174"/>
     <mergeCell ref="B192:E192"/>
     <mergeCell ref="B193:G193"/>
     <mergeCell ref="B200:G200"/>
@@ -14711,76 +14903,15 @@
     <mergeCell ref="B183:G183"/>
     <mergeCell ref="B184:E184"/>
     <mergeCell ref="B185:G185"/>
-    <mergeCell ref="B158:G158"/>
-    <mergeCell ref="B165:G165"/>
-    <mergeCell ref="B166:E166"/>
-    <mergeCell ref="B167:G167"/>
-    <mergeCell ref="B174:G174"/>
-    <mergeCell ref="B148:G148"/>
-    <mergeCell ref="B149:E149"/>
-    <mergeCell ref="B150:G150"/>
-    <mergeCell ref="B156:G156"/>
-    <mergeCell ref="B157:E157"/>
-    <mergeCell ref="B133:E133"/>
-    <mergeCell ref="B134:G134"/>
-    <mergeCell ref="B140:G140"/>
-    <mergeCell ref="B141:E141"/>
-    <mergeCell ref="B142:G142"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="A16:G16"/>
-    <mergeCell ref="A17:G17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B38:G38"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="B31:G31"/>
-    <mergeCell ref="B36:G36"/>
-    <mergeCell ref="B37:E37"/>
-    <mergeCell ref="B58:G58"/>
-    <mergeCell ref="B43:G43"/>
-    <mergeCell ref="B44:E44"/>
-    <mergeCell ref="B45:G45"/>
-    <mergeCell ref="B49:G49"/>
-    <mergeCell ref="B50:E50"/>
-    <mergeCell ref="B51:G51"/>
-    <mergeCell ref="B56:G56"/>
-    <mergeCell ref="B57:E57"/>
-    <mergeCell ref="B81:G81"/>
-    <mergeCell ref="B63:G63"/>
-    <mergeCell ref="B72:E72"/>
-    <mergeCell ref="B73:G73"/>
-    <mergeCell ref="B79:G79"/>
-    <mergeCell ref="B80:E80"/>
-    <mergeCell ref="B64:E64"/>
-    <mergeCell ref="B65:G65"/>
-    <mergeCell ref="B71:G71"/>
-    <mergeCell ref="B96:E96"/>
-    <mergeCell ref="B97:G97"/>
-    <mergeCell ref="B103:G103"/>
-    <mergeCell ref="B87:G87"/>
-    <mergeCell ref="B88:E88"/>
-    <mergeCell ref="B89:G89"/>
-    <mergeCell ref="B95:G95"/>
-    <mergeCell ref="B112:E112"/>
-    <mergeCell ref="B113:G113"/>
-    <mergeCell ref="B117:G117"/>
-    <mergeCell ref="B104:E104"/>
-    <mergeCell ref="B105:G105"/>
-    <mergeCell ref="B111:G111"/>
-    <mergeCell ref="B132:G132"/>
-    <mergeCell ref="B118:E118"/>
-    <mergeCell ref="B119:G119"/>
-    <mergeCell ref="B124:G124"/>
-    <mergeCell ref="B125:E125"/>
-    <mergeCell ref="B126:G126"/>
+    <mergeCell ref="B216:G216"/>
+    <mergeCell ref="B201:E201"/>
+    <mergeCell ref="B202:G202"/>
+    <mergeCell ref="B209:G209"/>
+    <mergeCell ref="B210:E210"/>
+    <mergeCell ref="B211:G211"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" showErrorMessage="1" promptTitle="Valid values include:" prompt="_x000a_" sqref="F367:F369 F374:F380 F593:F595 F583:F588 F385:F394 F399:F402 F407:F412 F417:F425 F430:F439 F444:F454 F459:F469 F485:F491 F513:F515 F474:F480 F496:F502 F507:F508 F520:F526 F531:F537 F553:F555 F542:F548 F560:F563 F568:F570 F575:F578 F213:F215 F204:F208 F195:F199 F187:F190 F178:F182 F169:F173 F160:F164 F152:F155 F144:F147 F136:F139 F128:F131 F121:F123 F115:F116 F99:F102 F91:F94 F83:F86 F60:F62 F53:F55 F47:F49 F33:F35 F40:F42 F26:F28 F75:F78 F67:F70 F107:F110 F21">
+    <dataValidation type="list" showErrorMessage="1" promptTitle="Valid values include:" prompt="_x000a_" sqref="F367:F369 F374:F380 F593:F595 F583:F588 F385:F394 F399:F402 F407:F412 F417:F425 F430:F439 F444:F454 F459:F469 F485:F491 F513:F515 F474:F480 F496:F502 F507:F508 F520:F526 F531:F537 F553:F555 F542:F548 F560:F563 F568:F570 F575:F578 F213:F215 F204:F208 F195:F199 F187:F190 F178:F182 F169:F173 F160:F164 F152:F155 F144:F147 F136:F139 F128:F131 F121:F123 F115:F116 F99:F102 F91:F94 F83:F86 F60:F62 F53:F55 F47:F49 F33:F35 F40:F42 F26:F28 F75:F78 F67:F70 F107:F110 F21" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"Pass, Fail, Blocked"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>